<commit_message>
fix: Nueva propuesta query expuestos autonomia
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED61C7AB-790E-4C44-B780-E808154BAF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09DDE73-77DB-524A-B514-22D35501D9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" tabRatio="844" activeTab="5" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" tabRatio="844" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="add_spe_Canal-Poliza" sheetId="8" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="add_s_Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
     <sheet name="CODS" sheetId="6" r:id="rId7"/>
     <sheet name="Fechas" sheetId="13" r:id="rId8"/>
-    <sheet name="add_s_SAP_Sinis_Ced" sheetId="39" r:id="rId9"/>
+    <sheet name="add_s_SAP_Sinis_Ced" sheetId="41" r:id="rId9"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId10"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="21" r:id="rId11"/>
     <sheet name="Gastos_Expedicion" sheetId="18" r:id="rId12"/>
@@ -52697,7 +52697,7 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -53770,10 +53770,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D3B91C-86A8-3748-B2F4-DFE901E6AB3E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29841E4A-C95D-DC46-8CB5-412D434AC28A}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -56199,6 +56201,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
@@ -56211,23 +56222,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F504A30D0A8B7C48AC3312637B06038A" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18aa81df5b435925a4ef391b68c25b4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="df0aad82-cca9-4ab3-a26b-b2d93ab652bf" xmlns:ns3="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019c64929386a1d9ec4afd0363aaee9d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -56499,7 +56494,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -56517,23 +56527,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -56551,4 +56545,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor: Separacion y simplificacion queries siniestros
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,32 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09DDE73-77DB-524A-B514-22D35501D9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B802A263-2DC9-824A-ABBD-5EF2ECF664D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" tabRatio="844" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="add_spe_Canal-Poliza" sheetId="8" r:id="rId1"/>
-    <sheet name="add_spe_Canal-Canal" sheetId="12" r:id="rId2"/>
-    <sheet name="add_spe_Canal-Sucursal" sheetId="9" r:id="rId3"/>
-    <sheet name="add_spe_Amparos" sheetId="1" r:id="rId4"/>
-    <sheet name="add_s_Atipicos" sheetId="14" r:id="rId5"/>
-    <sheet name="add_s_Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
+    <sheet name="add_pe_Canal-Poliza" sheetId="8" r:id="rId1"/>
+    <sheet name="add_pe_Canal-Canal" sheetId="12" r:id="rId2"/>
+    <sheet name="add_pe_Canal-Sucursal" sheetId="9" r:id="rId3"/>
+    <sheet name="add_pe_Amparos" sheetId="1" r:id="rId4"/>
+    <sheet name="Atipicos" sheetId="14" r:id="rId5"/>
+    <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
     <sheet name="CODS" sheetId="6" r:id="rId7"/>
     <sheet name="Fechas" sheetId="13" r:id="rId8"/>
-    <sheet name="add_s_SAP_Sinis_Ced" sheetId="41" r:id="rId9"/>
+    <sheet name="SAP_Sinis_Ced" sheetId="50" r:id="rId9"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId10"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="21" r:id="rId11"/>
     <sheet name="Gastos_Expedicion" sheetId="18" r:id="rId12"/>
     <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">add_s_Atipicos!$A$1:$G$1063</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">add_s_Inc_Ced_Atipicos!$A$1:$M$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">add_spe_Amparos!$A$1:$G$223</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'add_spe_Canal-Poliza'!$B$1:$H$43</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'add_spe_Canal-Sucursal'!$C$1:$H$2126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">add_pe_Amparos!$A$1:$G$223</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'add_pe_Canal-Poliza'!$B$1:$H$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'add_pe_Canal-Sucursal'!$C$1:$H$2126</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Amparos_Negocio_083!$A$1:$B$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Atipicos!$A$1:$G$1063</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Inc_Ced_Atipicos!$A$1:$M$29</definedName>
   </definedNames>
   <calcPr calcId="191028" concurrentManualCount="12"/>
   <extLst>
@@ -53770,11 +53770,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29841E4A-C95D-DC46-8CB5-412D434AC28A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430C109C-BE57-5A4E-A889-6774DB201E5C}">
   <dimension ref="A1:E500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -56201,28 +56201,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F504A30D0A8B7C48AC3312637B06038A" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18aa81df5b435925a4ef391b68c25b4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="df0aad82-cca9-4ab3-a26b-b2d93ab652bf" xmlns:ns3="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019c64929386a1d9ec4afd0363aaee9d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -56494,6 +56472,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <Application xmlns="http://www.sap.com/cof/excel/application">
   <Version>2</Version>
@@ -56502,9 +56502,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
+    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -56528,21 +56540,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
-    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fix: Reconocer si un query es de siniestros, primas, o expuestos
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DB7886-0F04-6245-8CA4-EB5572247080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3DD2D5-ADBD-E645-AA3B-81E89F756D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33980" yWindow="1820" windowWidth="30240" windowHeight="17380" tabRatio="844" activeTab="5" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="844" activeTab="3" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="add_pe_Canal-Poliza" sheetId="8" r:id="rId1"/>
     <sheet name="add_pe_Canal-Canal" sheetId="12" r:id="rId2"/>
     <sheet name="add_pe_Canal-Sucursal" sheetId="9" r:id="rId3"/>
-    <sheet name="add_pe_Amparos" sheetId="1" r:id="rId4"/>
+    <sheet name="add_e_Amparos" sheetId="1" r:id="rId4"/>
     <sheet name="Atipicos" sheetId="14" r:id="rId5"/>
     <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
     <sheet name="CODS" sheetId="6" r:id="rId7"/>
@@ -28,7 +28,7 @@
     <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">add_pe_Amparos!$A$1:$G$223</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">add_e_Amparos!$A$1:$G$223</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'add_pe_Canal-Poliza'!$B$1:$H$43</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'add_pe_Canal-Sucursal'!$C$1:$H$2126</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Amparos_Negocio_083!$A$1:$B$80</definedName>
@@ -21910,8 +21910,8 @@
   </sheetPr>
   <dimension ref="A1:G233"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -52694,7 +52694,7 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -56196,28 +56196,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F504A30D0A8B7C48AC3312637B06038A" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18aa81df5b435925a4ef391b68c25b4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="df0aad82-cca9-4ab3-a26b-b2d93ab652bf" xmlns:ns3="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019c64929386a1d9ec4afd0363aaee9d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -56489,6 +56467,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <Application xmlns="http://www.sap.com/cof/excel/application">
   <Version>2</Version>
@@ -56497,9 +56497,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
+    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -56523,21 +56535,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
-    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Leer primas de SAP para cuadre cedido autonomia
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3DD2D5-ADBD-E645-AA3B-81E89F756D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1A6AE9-3B5C-804E-B7EE-D7430FADE382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="844" activeTab="3" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="844" firstSheet="2" activeTab="11" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="add_pe_Canal-Poliza" sheetId="8" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="SAP_Sinis_Ced" sheetId="64" r:id="rId9"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId10"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="21" r:id="rId11"/>
-    <sheet name="Gastos_Expedicion" sheetId="18" r:id="rId12"/>
+    <sheet name="add_p_Gastos_Expedicion" sheetId="18" r:id="rId12"/>
     <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId13"/>
   </sheets>
   <definedNames>
@@ -6338,9 +6338,7 @@
   <sheetPr codeName="Hoja12"/>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21910,7 +21908,7 @@
   </sheetPr>
   <dimension ref="A1:G233"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -56468,16 +56466,10 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -56490,10 +56482,16 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -56517,6 +56515,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -56532,20 +56546,4 @@
     <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor: Reorganizar y simplificar constantes y parametros
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51175DDF-80CA-8F4C-8251-45B7098022DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDC443F-BE36-B24A-8255-01125EA373DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="844" activeTab="9" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="844" activeTab="7" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="add_pe_Canal-Poliza" sheetId="8" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Atipicos" sheetId="14" r:id="rId5"/>
     <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
     <sheet name="CODS" sheetId="6" r:id="rId7"/>
-    <sheet name="Fechas" sheetId="13" r:id="rId8"/>
+    <sheet name="Parametros" sheetId="13" r:id="rId8"/>
     <sheet name="add_p_SAP_Primas_Ced" sheetId="77" r:id="rId9"/>
     <sheet name="SAP_Sinis_Ced" sheetId="76" r:id="rId10"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId11"/>
@@ -36,7 +36,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Atipicos!$A$1:$G$1063</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Inc_Ced_Atipicos!$A$1:$M$29</definedName>
   </definedNames>
-  <calcPr calcId="191028" concurrentManualCount="12"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7813" uniqueCount="1332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7799" uniqueCount="1325">
   <si>
     <t>Amparo_Desc</t>
   </si>
@@ -3842,39 +3842,9 @@
     <t>Dia subida reaseguro Teradata</t>
   </si>
   <si>
-    <t>Tipo análisis</t>
-  </si>
-  <si>
     <t>Entremes</t>
   </si>
   <si>
-    <t>Correr teradata siniestros</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Correr teradata primas</t>
-  </si>
-  <si>
-    <t>Correr teradata expuestos</t>
-  </si>
-  <si>
-    <t>Generar controles siniestros</t>
-  </si>
-  <si>
-    <t>Generar controles primas</t>
-  </si>
-  <si>
-    <t>Generar controles expuestos</t>
-  </si>
-  <si>
-    <t>Cuadre contable siniestros</t>
-  </si>
-  <si>
-    <t>Cuadre contable primas</t>
-  </si>
-  <si>
     <t>codigo_op</t>
   </si>
   <si>
@@ -4053,6 +4023,15 @@
   </si>
   <si>
     <t>prima_cedida</t>
+  </si>
+  <si>
+    <t>Negocio</t>
+  </si>
+  <si>
+    <t>Autonomia</t>
+  </si>
+  <si>
+    <t>Tipo analisis</t>
   </si>
 </sst>
 </file>
@@ -6061,7 +6040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B9D2FB-F2C1-8E4B-9495-FD4B59359134}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -6069,19 +6048,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="50" t="s">
-        <v>1272</v>
+        <v>1262</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>1273</v>
+        <v>1263</v>
       </c>
       <c r="C1" t="s">
-        <v>1274</v>
+        <v>1264</v>
       </c>
       <c r="D1" t="s">
-        <v>1275</v>
+        <v>1265</v>
       </c>
       <c r="E1" t="s">
-        <v>1276</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -6089,7 +6068,7 @@
         <v>1092</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>1277</v>
+        <v>1267</v>
       </c>
       <c r="C2">
         <v>202405</v>
@@ -6106,7 +6085,7 @@
         <v>1092</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>1278</v>
+        <v>1268</v>
       </c>
       <c r="C3">
         <v>202405</v>
@@ -6123,7 +6102,7 @@
         <v>1092</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>1279</v>
+        <v>1269</v>
       </c>
       <c r="C4">
         <v>202405</v>
@@ -6140,7 +6119,7 @@
         <v>1092</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>1280</v>
+        <v>1270</v>
       </c>
       <c r="C5">
         <v>202405</v>
@@ -6157,7 +6136,7 @@
         <v>1092</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>1281</v>
+        <v>1271</v>
       </c>
       <c r="C6">
         <v>202405</v>
@@ -6174,7 +6153,7 @@
         <v>1092</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>1282</v>
+        <v>1272</v>
       </c>
       <c r="C7">
         <v>202405</v>
@@ -6191,7 +6170,7 @@
         <v>1092</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>1283</v>
+        <v>1273</v>
       </c>
       <c r="C8">
         <v>202405</v>
@@ -6208,7 +6187,7 @@
         <v>1092</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>1284</v>
+        <v>1274</v>
       </c>
       <c r="C9">
         <v>202405</v>
@@ -6225,7 +6204,7 @@
         <v>1092</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>1285</v>
+        <v>1275</v>
       </c>
       <c r="C10">
         <v>202405</v>
@@ -6242,7 +6221,7 @@
         <v>1092</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>1286</v>
+        <v>1276</v>
       </c>
       <c r="C11">
         <v>202405</v>
@@ -6259,7 +6238,7 @@
         <v>1092</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>1287</v>
+        <v>1277</v>
       </c>
       <c r="C12">
         <v>202405</v>
@@ -6276,7 +6255,7 @@
         <v>1092</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>1288</v>
+        <v>1278</v>
       </c>
       <c r="C13">
         <v>202405</v>
@@ -6293,7 +6272,7 @@
         <v>1092</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>1289</v>
+        <v>1279</v>
       </c>
       <c r="C14">
         <v>202405</v>
@@ -6310,7 +6289,7 @@
         <v>1092</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>1290</v>
+        <v>1280</v>
       </c>
       <c r="C15">
         <v>202405</v>
@@ -6327,7 +6306,7 @@
         <v>1092</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>1291</v>
+        <v>1281</v>
       </c>
       <c r="C16">
         <v>202405</v>
@@ -6344,7 +6323,7 @@
         <v>1092</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>1292</v>
+        <v>1282</v>
       </c>
       <c r="C17">
         <v>202405</v>
@@ -6361,7 +6340,7 @@
         <v>1092</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>1293</v>
+        <v>1283</v>
       </c>
       <c r="C18">
         <v>202405</v>
@@ -6378,7 +6357,7 @@
         <v>1092</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>1294</v>
+        <v>1284</v>
       </c>
       <c r="C19">
         <v>202405</v>
@@ -6395,7 +6374,7 @@
         <v>1092</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>1295</v>
+        <v>1285</v>
       </c>
       <c r="C20">
         <v>202405</v>
@@ -6412,7 +6391,7 @@
         <v>1092</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>1296</v>
+        <v>1286</v>
       </c>
       <c r="C21">
         <v>202405</v>
@@ -6429,7 +6408,7 @@
         <v>1092</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>1297</v>
+        <v>1287</v>
       </c>
       <c r="C22">
         <v>202405</v>
@@ -6497,7 +6476,7 @@
         <v>154</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>1298</v>
+        <v>1288</v>
       </c>
       <c r="C26">
         <v>202405</v>
@@ -6514,7 +6493,7 @@
         <v>154</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>1299</v>
+        <v>1289</v>
       </c>
       <c r="C27">
         <v>202405</v>
@@ -6531,7 +6510,7 @@
         <v>154</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>1300</v>
+        <v>1290</v>
       </c>
       <c r="C28">
         <v>202405</v>
@@ -6548,7 +6527,7 @@
         <v>154</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>1301</v>
+        <v>1291</v>
       </c>
       <c r="C29">
         <v>202405</v>
@@ -6582,7 +6561,7 @@
         <v>154</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>1302</v>
+        <v>1292</v>
       </c>
       <c r="C31">
         <v>202405</v>
@@ -56161,10 +56140,10 @@
   <sheetPr codeName="Hoja7">
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="163" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -56191,88 +56170,32 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>1261</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>1262</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>1263</v>
+        <v>1322</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>1264</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>1265</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
-        <v>1266</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
-        <v>1268</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
-        <v>1270</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
-        <v>1271</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
         <v>1260</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B5" s="18">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B11" xr:uid="{96B20A32-B83E-7549-845E-67D7BD66CE0A}">
-      <formula1>"SI,NO"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{96B20A32-B83E-7549-845E-67D7BD66CE0A}">
+      <formula1>"ARL,Autonomia,Empresariales,Movilidad,Salud,SOAT"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{E9389E5D-9C3E-C249-8951-99AB1ED1B6C7}">
       <formula1>"Triangulos,Entremes"</formula1>
@@ -56297,37 +56220,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="50" t="s">
-        <v>1272</v>
+        <v>1262</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>1273</v>
+        <v>1263</v>
       </c>
       <c r="C1" t="s">
-        <v>1274</v>
+        <v>1264</v>
       </c>
       <c r="D1" t="s">
-        <v>1303</v>
+        <v>1293</v>
       </c>
       <c r="E1" t="s">
-        <v>1304</v>
+        <v>1294</v>
       </c>
       <c r="F1" t="s">
-        <v>1305</v>
+        <v>1295</v>
       </c>
       <c r="G1" t="s">
-        <v>1306</v>
+        <v>1296</v>
       </c>
       <c r="H1" t="s">
-        <v>1307</v>
+        <v>1297</v>
       </c>
       <c r="I1" t="s">
-        <v>1308</v>
+        <v>1298</v>
       </c>
       <c r="J1" t="s">
-        <v>1330</v>
+        <v>1320</v>
       </c>
       <c r="K1" t="s">
-        <v>1331</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -56335,7 +56258,7 @@
         <v>1092</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>1277</v>
+        <v>1267</v>
       </c>
       <c r="C2">
         <v>202405</v>
@@ -56370,7 +56293,7 @@
         <v>1092</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>1309</v>
+        <v>1299</v>
       </c>
       <c r="C3">
         <v>202405</v>
@@ -56405,7 +56328,7 @@
         <v>1092</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>1278</v>
+        <v>1268</v>
       </c>
       <c r="C4">
         <v>202405</v>
@@ -56440,7 +56363,7 @@
         <v>1092</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>1310</v>
+        <v>1300</v>
       </c>
       <c r="C5">
         <v>202405</v>
@@ -56475,7 +56398,7 @@
         <v>1092</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>1279</v>
+        <v>1269</v>
       </c>
       <c r="C6">
         <v>202405</v>
@@ -56510,7 +56433,7 @@
         <v>1092</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>1280</v>
+        <v>1270</v>
       </c>
       <c r="C7">
         <v>202405</v>
@@ -56545,7 +56468,7 @@
         <v>1092</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>1281</v>
+        <v>1271</v>
       </c>
       <c r="C8">
         <v>202405</v>
@@ -56580,7 +56503,7 @@
         <v>1092</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>1282</v>
+        <v>1272</v>
       </c>
       <c r="C9">
         <v>202405</v>
@@ -56615,7 +56538,7 @@
         <v>1092</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>1283</v>
+        <v>1273</v>
       </c>
       <c r="C10">
         <v>202405</v>
@@ -56650,7 +56573,7 @@
         <v>1092</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>1284</v>
+        <v>1274</v>
       </c>
       <c r="C11">
         <v>202405</v>
@@ -56685,7 +56608,7 @@
         <v>1092</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>1285</v>
+        <v>1275</v>
       </c>
       <c r="C12">
         <v>202405</v>
@@ -56720,7 +56643,7 @@
         <v>1092</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>1286</v>
+        <v>1276</v>
       </c>
       <c r="C13">
         <v>202405</v>
@@ -56755,7 +56678,7 @@
         <v>1092</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>1287</v>
+        <v>1277</v>
       </c>
       <c r="C14">
         <v>202405</v>
@@ -56790,7 +56713,7 @@
         <v>1092</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>1288</v>
+        <v>1278</v>
       </c>
       <c r="C15">
         <v>202405</v>
@@ -56825,7 +56748,7 @@
         <v>1092</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>1289</v>
+        <v>1279</v>
       </c>
       <c r="C16">
         <v>202405</v>
@@ -56860,7 +56783,7 @@
         <v>1092</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>1290</v>
+        <v>1280</v>
       </c>
       <c r="C17">
         <v>202405</v>
@@ -56895,7 +56818,7 @@
         <v>1092</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>1291</v>
+        <v>1281</v>
       </c>
       <c r="C18">
         <v>202405</v>
@@ -56930,7 +56853,7 @@
         <v>1092</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>1292</v>
+        <v>1282</v>
       </c>
       <c r="C19">
         <v>202405</v>
@@ -56965,7 +56888,7 @@
         <v>1092</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>1293</v>
+        <v>1283</v>
       </c>
       <c r="C20">
         <v>202405</v>
@@ -57000,7 +56923,7 @@
         <v>1092</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>1311</v>
+        <v>1301</v>
       </c>
       <c r="C21">
         <v>202405</v>
@@ -57035,7 +56958,7 @@
         <v>1092</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>1294</v>
+        <v>1284</v>
       </c>
       <c r="C22">
         <v>202405</v>
@@ -57070,7 +56993,7 @@
         <v>1092</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>1295</v>
+        <v>1285</v>
       </c>
       <c r="C23">
         <v>202405</v>
@@ -57105,7 +57028,7 @@
         <v>1092</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>1312</v>
+        <v>1302</v>
       </c>
       <c r="C24">
         <v>202405</v>
@@ -57245,7 +57168,7 @@
         <v>1092</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>1313</v>
+        <v>1303</v>
       </c>
       <c r="C28">
         <v>202405</v>
@@ -57280,7 +57203,7 @@
         <v>1092</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>1296</v>
+        <v>1286</v>
       </c>
       <c r="C29">
         <v>202405</v>
@@ -57315,7 +57238,7 @@
         <v>1092</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>1297</v>
+        <v>1287</v>
       </c>
       <c r="C30">
         <v>202405</v>
@@ -57350,7 +57273,7 @@
         <v>1092</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>1314</v>
+        <v>1304</v>
       </c>
       <c r="C31">
         <v>202405</v>
@@ -57385,7 +57308,7 @@
         <v>1092</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>1315</v>
+        <v>1305</v>
       </c>
       <c r="C32">
         <v>202405</v>
@@ -57420,7 +57343,7 @@
         <v>1092</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>1316</v>
+        <v>1306</v>
       </c>
       <c r="C33">
         <v>202405</v>
@@ -57455,7 +57378,7 @@
         <v>1092</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>1317</v>
+        <v>1307</v>
       </c>
       <c r="C34">
         <v>202405</v>
@@ -57490,7 +57413,7 @@
         <v>1092</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>1318</v>
+        <v>1308</v>
       </c>
       <c r="C35">
         <v>202405</v>
@@ -57560,7 +57483,7 @@
         <v>154</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>1319</v>
+        <v>1309</v>
       </c>
       <c r="C37">
         <v>202405</v>
@@ -57595,7 +57518,7 @@
         <v>154</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>1320</v>
+        <v>1310</v>
       </c>
       <c r="C38">
         <v>202405</v>
@@ -57630,7 +57553,7 @@
         <v>154</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>1321</v>
+        <v>1311</v>
       </c>
       <c r="C39">
         <v>202405</v>
@@ -57700,7 +57623,7 @@
         <v>154</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>1322</v>
+        <v>1312</v>
       </c>
       <c r="C41">
         <v>202405</v>
@@ -57875,7 +57798,7 @@
         <v>154</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>1323</v>
+        <v>1313</v>
       </c>
       <c r="C46">
         <v>202405</v>
@@ -57910,7 +57833,7 @@
         <v>154</v>
       </c>
       <c r="B47" s="50" t="s">
-        <v>1324</v>
+        <v>1314</v>
       </c>
       <c r="C47">
         <v>202405</v>
@@ -57945,7 +57868,7 @@
         <v>154</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>1298</v>
+        <v>1288</v>
       </c>
       <c r="C48">
         <v>202405</v>
@@ -57980,7 +57903,7 @@
         <v>154</v>
       </c>
       <c r="B49" s="50" t="s">
-        <v>1299</v>
+        <v>1289</v>
       </c>
       <c r="C49">
         <v>202405</v>
@@ -58015,7 +57938,7 @@
         <v>154</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>1300</v>
+        <v>1290</v>
       </c>
       <c r="C50">
         <v>202405</v>
@@ -58050,7 +57973,7 @@
         <v>154</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>1325</v>
+        <v>1315</v>
       </c>
       <c r="C51">
         <v>202405</v>
@@ -58085,7 +58008,7 @@
         <v>154</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>1326</v>
+        <v>1316</v>
       </c>
       <c r="C52">
         <v>202405</v>
@@ -58120,7 +58043,7 @@
         <v>154</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>1327</v>
+        <v>1317</v>
       </c>
       <c r="C53">
         <v>202405</v>
@@ -58155,7 +58078,7 @@
         <v>154</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>1301</v>
+        <v>1291</v>
       </c>
       <c r="C54">
         <v>202405</v>
@@ -58225,7 +58148,7 @@
         <v>154</v>
       </c>
       <c r="B56" s="50" t="s">
-        <v>1302</v>
+        <v>1292</v>
       </c>
       <c r="C56">
         <v>202405</v>
@@ -58260,7 +58183,7 @@
         <v>154</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>1328</v>
+        <v>1318</v>
       </c>
       <c r="C57">
         <v>202405</v>
@@ -58295,7 +58218,7 @@
         <v>154</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>1329</v>
+        <v>1319</v>
       </c>
       <c r="C58">
         <v>202405</v>
@@ -60130,13 +60053,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <Application xmlns="http://www.sap.com/cof/excel/application">
   <Version>2</Version>
   <Revision>2.3.1.59180</Revision>
 </Application>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F504A30D0A8B7C48AC3312637B06038A" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18aa81df5b435925a4ef391b68c25b4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="df0aad82-cca9-4ab3-a26b-b2d93ab652bf" xmlns:ns3="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019c64929386a1d9ec4afd0363aaee9d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -60408,29 +60353,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
+    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
@@ -60438,7 +60387,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -60456,30 +60405,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
-    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: Corregir macros de preparar y guardar
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAB6786-1689-5848-8706-834443B3CBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDC2901-4743-2D4F-9220-E9BBD2106A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="844" firstSheet="4" activeTab="11" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="844" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="add_pe_Canal-Poliza" sheetId="8" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
     <sheet name="CODS" sheetId="6" r:id="rId7"/>
     <sheet name="Parametros" sheetId="13" r:id="rId8"/>
-    <sheet name="add_p_SAP_Primas_Ced" sheetId="87" r:id="rId9"/>
-    <sheet name="SAP_Sinis_Ced" sheetId="86" r:id="rId10"/>
+    <sheet name="add_p_SAP_Primas_Ced" sheetId="89" r:id="rId9"/>
+    <sheet name="SAP_Sinis_Ced" sheetId="88" r:id="rId10"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId11"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="21" r:id="rId12"/>
     <sheet name="add_p_Gastos_Expedicion" sheetId="18" r:id="rId13"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7709" uniqueCount="1278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7697" uniqueCount="1278">
   <si>
     <t>Amparo_Desc</t>
   </si>
@@ -3800,9 +3800,6 @@
     <t>Dia subida reaseguro Teradata</t>
   </si>
   <si>
-    <t>Entremes</t>
-  </si>
-  <si>
     <t>codigo_op</t>
   </si>
   <si>
@@ -3891,6 +3888,9 @@
   </si>
   <si>
     <t>apertura_reservas</t>
+  </si>
+  <si>
+    <t>Triangulos</t>
   </si>
 </sst>
 </file>
@@ -5896,7 +5896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8205C5-0977-A441-8E2E-E32FF0204A5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004C085E-46E1-AE40-8019-39D4C524091E}">
   <dimension ref="A1:E500"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5905,88 +5905,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="50" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>1248</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="C1" t="s">
         <v>1249</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1250</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1251</v>
       </c>
-      <c r="E1" t="s">
-        <v>1252</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2">
-        <v>202405</v>
-      </c>
-      <c r="D2">
-        <v>2109682582</v>
-      </c>
-      <c r="E2">
-        <v>-1377650651</v>
-      </c>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3">
-        <v>202405</v>
-      </c>
-      <c r="D3">
-        <v>4687639971</v>
-      </c>
-      <c r="E3">
-        <v>-603871447</v>
-      </c>
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>857</v>
-      </c>
-      <c r="C4">
-        <v>202405</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>2010597779</v>
-      </c>
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>870</v>
-      </c>
-      <c r="C5">
-        <v>202405</v>
-      </c>
-      <c r="D5">
-        <v>452206617</v>
-      </c>
-      <c r="E5">
-        <v>40427455</v>
-      </c>
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="50"/>
@@ -7994,16 +7942,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B1" s="40" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>1248</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>1249</v>
-      </c>
       <c r="D1" s="40" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="E1" s="40" t="s">
         <v>128</v>
@@ -8021,10 +7969,10 @@
         <v>1092</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D2" t="s">
         <v>1267</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1268</v>
       </c>
       <c r="E2" t="s">
         <v>175</v>
@@ -8068,7 +8016,7 @@
         <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>161</v>
@@ -8090,7 +8038,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>161</v>
@@ -8112,7 +8060,7 @@
         <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>1105</v>
@@ -8133,7 +8081,7 @@
         <v>857</v>
       </c>
       <c r="D7" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="E7" t="s">
         <v>175</v>
@@ -8154,7 +8102,7 @@
         <v>857</v>
       </c>
       <c r="D8" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="E8" t="s">
         <v>175</v>
@@ -8175,7 +8123,7 @@
         <v>1095</v>
       </c>
       <c r="D9" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E9" t="s">
         <v>175</v>
@@ -8196,7 +8144,7 @@
         <v>1095</v>
       </c>
       <c r="D10" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E10" t="s">
         <v>175</v>
@@ -8217,7 +8165,7 @@
         <v>870</v>
       </c>
       <c r="D11" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="E11" t="s">
         <v>175</v>
@@ -8238,7 +8186,7 @@
         <v>134</v>
       </c>
       <c r="D12" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>161</v>
@@ -8256,10 +8204,10 @@
         <v>154</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="D13" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="E13" t="s">
         <v>175</v>
@@ -8277,10 +8225,10 @@
         <v>154</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="D14" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="E14" t="s">
         <v>175</v>
@@ -8304,7 +8252,7 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -8320,16 +8268,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B1" s="40" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>1248</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>1249</v>
-      </c>
       <c r="D1" s="40" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="E1" s="40" t="s">
         <v>128</v>
@@ -8347,10 +8295,10 @@
         <v>1092</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D2" t="s">
         <v>1267</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1268</v>
       </c>
       <c r="E2" t="s">
         <v>175</v>
@@ -8392,7 +8340,7 @@
         <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>161</v>
@@ -8413,7 +8361,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>161</v>
@@ -8434,7 +8382,7 @@
         <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>1105</v>
@@ -8455,7 +8403,7 @@
         <v>857</v>
       </c>
       <c r="D7" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="E7" t="s">
         <v>175</v>
@@ -8476,7 +8424,7 @@
         <v>857</v>
       </c>
       <c r="D8" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="E8" t="s">
         <v>175</v>
@@ -8497,7 +8445,7 @@
         <v>1095</v>
       </c>
       <c r="D9" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E9" t="s">
         <v>175</v>
@@ -8518,7 +8466,7 @@
         <v>1095</v>
       </c>
       <c r="D10" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E10" t="s">
         <v>175</v>
@@ -8539,7 +8487,7 @@
         <v>870</v>
       </c>
       <c r="D11" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="E11" t="s">
         <v>175</v>
@@ -8560,7 +8508,7 @@
         <v>134</v>
       </c>
       <c r="D12" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>161</v>
@@ -8578,10 +8526,10 @@
         <v>154</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="D13" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="E13" t="s">
         <v>175</v>
@@ -8599,10 +8547,10 @@
         <v>154</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="D14" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="E14" t="s">
         <v>175</v>
@@ -55931,7 +55879,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="163" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -55945,7 +55893,7 @@
         <v>187</v>
       </c>
       <c r="B1" s="18">
-        <v>201401</v>
+        <v>201409</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -55953,23 +55901,23 @@
         <v>188</v>
       </c>
       <c r="B2" s="18">
-        <v>202405</v>
+        <v>202409</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>1247</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>1263</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>1264</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -55997,46 +55945,46 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7255843-5FFA-434B-9090-9C8D9886AB57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03D246F-9C5A-DF4D-ACF9-78F78DD4A221}">
   <dimension ref="A1:K500"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="50" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>1248</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="C1" t="s">
         <v>1249</v>
       </c>
-      <c r="C1" t="s">
-        <v>1250</v>
-      </c>
       <c r="D1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E1" t="s">
         <v>1253</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1254</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1255</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1256</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>1257</v>
       </c>
-      <c r="I1" t="s">
-        <v>1258</v>
-      </c>
       <c r="J1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="K1" t="s">
         <v>1261</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1262</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -56047,28 +55995,28 @@
         <v>96</v>
       </c>
       <c r="C2">
-        <v>202405</v>
+        <v>202409</v>
       </c>
       <c r="D2">
-        <v>192294403</v>
+        <v>89447254</v>
       </c>
       <c r="E2">
-        <v>192294403</v>
+        <v>89447254</v>
       </c>
       <c r="F2">
-        <v>238961798</v>
+        <v>89250257</v>
       </c>
       <c r="G2">
-        <v>238961798</v>
+        <v>89250257</v>
       </c>
       <c r="H2">
-        <v>1079189</v>
+        <v>-196997</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1079189</v>
+        <v>-196997</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -56082,28 +56030,28 @@
         <v>857</v>
       </c>
       <c r="C3">
-        <v>202405</v>
+        <v>202409</v>
       </c>
       <c r="D3">
-        <v>649048977</v>
+        <v>262825624</v>
       </c>
       <c r="E3">
-        <v>649048977</v>
+        <v>262825624</v>
       </c>
       <c r="F3">
-        <v>667832512</v>
+        <v>195182259</v>
       </c>
       <c r="G3">
-        <v>667832512</v>
+        <v>195182259</v>
       </c>
       <c r="H3">
-        <v>15802349</v>
+        <v>-67643365</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>15802348</v>
+        <v>-67643365</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -56111,34 +56059,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="50" t="s">
-        <v>1092</v>
+        <v>154</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C4">
-        <v>202405</v>
+        <v>202409</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>28195596</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>28195596</v>
       </c>
       <c r="F4">
-        <v>-3236</v>
+        <v>27878914</v>
       </c>
       <c r="G4">
-        <v>-3236</v>
+        <v>27878914</v>
       </c>
       <c r="H4">
-        <v>-3236</v>
+        <v>-316682</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>-3236</v>
+        <v>-316682</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -56149,31 +56097,31 @@
         <v>154</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>1093</v>
+        <v>127</v>
       </c>
       <c r="C5">
-        <v>202405</v>
+        <v>202409</v>
       </c>
       <c r="D5">
-        <v>1870748294</v>
+        <v>31606380267</v>
       </c>
       <c r="E5">
-        <v>1870748294</v>
+        <v>31606380267</v>
       </c>
       <c r="F5">
-        <v>1919978149</v>
+        <v>31710120607</v>
       </c>
       <c r="G5">
-        <v>1919978149</v>
+        <v>31710120607</v>
       </c>
       <c r="H5">
-        <v>49229855</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>49229855</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -56184,34 +56132,34 @@
         <v>154</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="C6">
-        <v>202405</v>
+        <v>202409</v>
       </c>
       <c r="D6">
-        <v>42344253894</v>
+        <v>5997308438</v>
       </c>
       <c r="E6">
-        <v>39685492502</v>
+        <v>5997308438</v>
       </c>
       <c r="F6">
-        <v>42308634086</v>
+        <v>3961313085</v>
       </c>
       <c r="G6">
-        <v>39649872694</v>
+        <v>3961313085</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>-2035995353</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
+        <v>-2035995353</v>
+      </c>
+      <c r="K6">
         <v>0</v>
-      </c>
-      <c r="K6">
-        <v>2658761392</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -56219,34 +56167,34 @@
         <v>154</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>96</v>
+        <v>857</v>
       </c>
       <c r="C7">
-        <v>202405</v>
+        <v>202409</v>
       </c>
       <c r="D7">
-        <v>107386595529</v>
+        <v>543350914</v>
       </c>
       <c r="E7">
-        <v>106760244650</v>
+        <v>543350914</v>
       </c>
       <c r="F7">
-        <v>112574343474</v>
+        <v>329070507</v>
       </c>
       <c r="G7">
-        <v>111947992595</v>
+        <v>329070507</v>
       </c>
       <c r="H7">
-        <v>5237276415</v>
+        <v>-214280407</v>
       </c>
       <c r="I7">
-        <v>-49528472</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>5286804887</v>
+        <v>-214280407</v>
       </c>
       <c r="K7">
-        <v>626350879</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -56254,34 +56202,34 @@
         <v>154</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>857</v>
+        <v>1095</v>
       </c>
       <c r="C8">
-        <v>202405</v>
+        <v>202409</v>
       </c>
       <c r="D8">
-        <v>4745049696</v>
+        <v>158702644</v>
       </c>
       <c r="E8">
-        <v>3568934246</v>
+        <v>158702644</v>
       </c>
       <c r="F8">
-        <v>4940644366</v>
+        <v>79952918</v>
       </c>
       <c r="G8">
-        <v>3764528916</v>
+        <v>79952918</v>
       </c>
       <c r="H8">
-        <v>252289175</v>
+        <v>-78749726</v>
       </c>
       <c r="I8">
-        <v>-56694507</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>308983682</v>
+        <v>-78749726</v>
       </c>
       <c r="K8">
-        <v>1176115450</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -56289,31 +56237,31 @@
         <v>154</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>1095</v>
+        <v>1259</v>
       </c>
       <c r="C9">
-        <v>202405</v>
+        <v>202409</v>
       </c>
       <c r="D9">
-        <v>391499630</v>
+        <v>39177883</v>
       </c>
       <c r="E9">
-        <v>391499630</v>
+        <v>39177883</v>
       </c>
       <c r="F9">
-        <v>536319393</v>
+        <v>39177883</v>
       </c>
       <c r="G9">
-        <v>536319393</v>
+        <v>39177883</v>
       </c>
       <c r="H9">
-        <v>144819763</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>144819763</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -56324,105 +56272,43 @@
         <v>154</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>1259</v>
+        <v>870</v>
       </c>
       <c r="C10">
-        <v>202405</v>
+        <v>202409</v>
       </c>
       <c r="D10">
-        <v>184493561</v>
+        <v>1989447647</v>
       </c>
       <c r="E10">
-        <v>61917269</v>
+        <v>1989447647</v>
       </c>
       <c r="F10">
-        <v>185422938</v>
+        <v>750860221</v>
       </c>
       <c r="G10">
-        <v>62846646</v>
+        <v>750860221</v>
       </c>
       <c r="H10">
-        <v>2227041</v>
+        <v>-1238587426</v>
       </c>
       <c r="I10">
-        <v>-1297664</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>3524705</v>
+        <v>-1238587426</v>
       </c>
       <c r="K10">
-        <v>122576292</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>1260</v>
-      </c>
-      <c r="C11">
-        <v>202405</v>
-      </c>
-      <c r="D11">
-        <v>97581289</v>
-      </c>
-      <c r="E11">
-        <v>97581289</v>
-      </c>
-      <c r="F11">
-        <v>104286828</v>
-      </c>
-      <c r="G11">
-        <v>104286828</v>
-      </c>
-      <c r="H11">
-        <v>6705539</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>6705539</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>870</v>
-      </c>
-      <c r="C12">
-        <v>202405</v>
-      </c>
-      <c r="D12">
-        <v>1664317911</v>
-      </c>
-      <c r="E12">
-        <v>1201052360</v>
-      </c>
-      <c r="F12">
-        <v>1659229103</v>
-      </c>
-      <c r="G12">
-        <v>1195963552</v>
-      </c>
-      <c r="H12">
-        <v>47313945</v>
-      </c>
-      <c r="I12">
-        <v>-52402760</v>
-      </c>
-      <c r="J12">
-        <v>99716705</v>
-      </c>
-      <c r="K12">
-        <v>463265551</v>
-      </c>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="50"/>
@@ -58382,19 +58268,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F504A30D0A8B7C48AC3312637B06038A" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18aa81df5b435925a4ef391b68c25b4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="df0aad82-cca9-4ab3-a26b-b2d93ab652bf" xmlns:ns3="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019c64929386a1d9ec4afd0363aaee9d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -58666,14 +58539,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <Application xmlns="http://www.sap.com/cof/excel/application">
   <Version>2</Version>
   <Revision>2.3.1.59180</Revision>
 </Application>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -58682,25 +58555,20 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
-    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -58720,7 +58588,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
@@ -58728,10 +58596,28 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
+    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Agregar modos de guardar y traer todo
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDC2901-4743-2D4F-9220-E9BBD2106A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D39B5C8-43E5-1044-9551-41F8426362DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="844" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
@@ -21,8 +21,8 @@
     <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
     <sheet name="CODS" sheetId="6" r:id="rId7"/>
     <sheet name="Parametros" sheetId="13" r:id="rId8"/>
-    <sheet name="add_p_SAP_Primas_Ced" sheetId="89" r:id="rId9"/>
-    <sheet name="SAP_Sinis_Ced" sheetId="88" r:id="rId10"/>
+    <sheet name="add_p_SAP_Primas_Ced" sheetId="99" r:id="rId9"/>
+    <sheet name="SAP_Sinis_Ced" sheetId="98" r:id="rId10"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId11"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="21" r:id="rId12"/>
     <sheet name="add_p_Gastos_Expedicion" sheetId="18" r:id="rId13"/>
@@ -5896,7 +5896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004C085E-46E1-AE40-8019-39D4C524091E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F53E4FD9-C51F-CB4C-BA2D-7133714F4A7E}">
   <dimension ref="A1:E500"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -55945,7 +55945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03D246F-9C5A-DF4D-ACF9-78F78DD4A221}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7F909C-57A3-084A-8B74-B0948BBD5EFC}">
   <dimension ref="A1:K500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -58268,6 +58268,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F504A30D0A8B7C48AC3312637B06038A" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18aa81df5b435925a4ef391b68c25b4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="df0aad82-cca9-4ab3-a26b-b2d93ab652bf" xmlns:ns3="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019c64929386a1d9ec4afd0363aaee9d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -58539,23 +58546,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
@@ -58568,7 +58559,24 @@
 </p:properties>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -58588,23 +58596,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -58620,4 +58612,12 @@
     <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Modificar frontend para que solo use una ruta y llame al backend directamente cuando se presiona un boton
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE8848E-ED08-3541-A155-4CF090281596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFCCBA8-8531-FB42-B98A-BD679922BFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22560" windowHeight="17380" tabRatio="844" firstSheet="6" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22560" windowHeight="17380" tabRatio="844" firstSheet="3" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="add_pe_Canal-Poliza" sheetId="8" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId7"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="21" r:id="rId8"/>
-    <sheet name="add_p_SAP_Primas_Ced" sheetId="105" r:id="rId9"/>
+    <sheet name="add_p_SAP_Primas_Ced" sheetId="107" r:id="rId9"/>
     <sheet name="SAP_Sinis_Ced" sheetId="104" r:id="rId10"/>
     <sheet name="add_p_Gastos_Expedicion" sheetId="18" r:id="rId11"/>
     <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId12"/>
@@ -55175,11 +55175,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF84EF2E-D44F-9A46-AF7C-3F8D015E2EAC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A2B8D3-8697-8047-B90E-9EF188533867}">
   <dimension ref="A1:K500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57531,19 +57531,22 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F504A30D0A8B7C48AC3312637B06038A" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18aa81df5b435925a4ef391b68c25b4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="df0aad82-cca9-4ab3-a26b-b2d93ab652bf" xmlns:ns3="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019c64929386a1d9ec4afd0363aaee9d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -57815,41 +57818,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
-    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -57869,18 +57867,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
+    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Generar error si no se tiene informacion de cierres anteriores para el entremes
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFCCBA8-8531-FB42-B98A-BD679922BFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9DAD00-5E6F-2E41-972E-A631FCF651C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="22560" windowHeight="17380" tabRatio="844" firstSheet="3" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
@@ -21,8 +21,8 @@
     <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId7"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="21" r:id="rId8"/>
-    <sheet name="add_p_SAP_Primas_Ced" sheetId="107" r:id="rId9"/>
-    <sheet name="SAP_Sinis_Ced" sheetId="104" r:id="rId10"/>
+    <sheet name="SAP_Sinis_Ced" sheetId="109" r:id="rId9"/>
+    <sheet name="add_p_SAP_Primas_Ced" sheetId="108" r:id="rId10"/>
     <sheet name="add_p_Gastos_Expedicion" sheetId="18" r:id="rId11"/>
     <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId12"/>
   </sheets>
@@ -5574,14 +5574,15 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB02E36F-DD49-9D48-B31B-70A7C6ABE7EB}">
-  <dimension ref="A1:E500"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A129746-6CD1-624B-BD34-B413117965C4}">
+  <sheetPr codeName="Hoja7"/>
+  <dimension ref="A1:K500"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>1203</v>
       </c>
@@ -5592,186 +5593,397 @@
         <v>1229</v>
       </c>
       <c r="D1" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
       <c r="E1" t="s">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1208</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>1074</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="45">
-        <v>45627</v>
+      <c r="C2">
+        <v>202412</v>
       </c>
       <c r="D2">
-        <v>8824813</v>
+        <v>184648783</v>
       </c>
       <c r="E2">
-        <v>-6875556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>184648783</v>
+      </c>
+      <c r="F2">
+        <v>203895741</v>
+      </c>
+      <c r="G2">
+        <v>203895741</v>
+      </c>
+      <c r="H2">
+        <v>19246958</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>19246958</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
         <v>1074</v>
       </c>
       <c r="B3" s="44" t="s">
         <v>839</v>
       </c>
-      <c r="C3" s="45">
-        <v>45627</v>
+      <c r="C3">
+        <v>202412</v>
       </c>
       <c r="D3">
+        <v>662347303</v>
+      </c>
+      <c r="E3">
+        <v>662347303</v>
+      </c>
+      <c r="F3">
+        <v>694786204</v>
+      </c>
+      <c r="G3">
+        <v>694786204</v>
+      </c>
+      <c r="H3">
+        <v>36305051</v>
+      </c>
+      <c r="I3">
+        <v>593</v>
+      </c>
+      <c r="J3">
+        <v>36304458</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B4" s="44" t="s">
         <v>1075</v>
       </c>
-      <c r="C4" s="45">
-        <v>45627</v>
+      <c r="C4">
+        <v>202412</v>
       </c>
       <c r="D4">
+        <v>1427498894</v>
+      </c>
+      <c r="E4">
+        <v>1427498894</v>
+      </c>
+      <c r="F4">
+        <v>1432785215</v>
+      </c>
+      <c r="G4">
+        <v>1432785215</v>
+      </c>
+      <c r="H4">
+        <v>5286321</v>
+      </c>
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="J4">
+        <v>5286321</v>
+      </c>
+      <c r="K4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="45">
-        <v>45627</v>
+      <c r="C5">
+        <v>202412</v>
       </c>
       <c r="D5">
-        <v>574118578</v>
+        <v>37620549295</v>
       </c>
       <c r="E5">
-        <v>3878153423</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34615671489</v>
+      </c>
+      <c r="F5">
+        <v>37727865277</v>
+      </c>
+      <c r="G5">
+        <v>34722987471</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>3004877806</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B6" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="45">
-        <v>45627</v>
+      <c r="C6">
+        <v>202412</v>
       </c>
       <c r="D6">
-        <v>4952998587</v>
+        <v>179132945472</v>
       </c>
       <c r="E6">
-        <v>-4070914402</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>179129728394</v>
+      </c>
+      <c r="F6">
+        <v>157701048874</v>
+      </c>
+      <c r="G6">
+        <v>157697831796</v>
+      </c>
+      <c r="H6">
+        <v>-21234067395</v>
+      </c>
+      <c r="I6">
+        <v>-197829203</v>
+      </c>
+      <c r="J6">
+        <v>-21036238192</v>
+      </c>
+      <c r="K6">
+        <v>3217078</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B7" s="44" t="s">
         <v>839</v>
       </c>
-      <c r="C7" s="45">
-        <v>45627</v>
+      <c r="C7">
+        <v>202412</v>
       </c>
       <c r="D7">
-        <v>132659301</v>
+        <v>4564533939</v>
       </c>
       <c r="E7">
-        <v>-134705661</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3488760438</v>
+      </c>
+      <c r="F7">
+        <v>4718335471</v>
+      </c>
+      <c r="G7">
+        <v>3642561970</v>
+      </c>
+      <c r="H7">
+        <v>429469879</v>
+      </c>
+      <c r="I7">
+        <v>-275668347</v>
+      </c>
+      <c r="J7">
+        <v>705138226</v>
+      </c>
+      <c r="K7">
+        <v>1075773501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B8" s="44" t="s">
         <v>1077</v>
       </c>
-      <c r="C8" s="45">
-        <v>45627</v>
+      <c r="C8">
+        <v>202412</v>
       </c>
       <c r="D8">
+        <v>371614941</v>
+      </c>
+      <c r="E8">
+        <v>371614941</v>
+      </c>
+      <c r="F8">
+        <v>512133717</v>
+      </c>
+      <c r="G8">
+        <v>512133717</v>
+      </c>
+      <c r="H8">
+        <v>140518776</v>
+      </c>
+      <c r="I8">
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="J8">
+        <v>140518776</v>
+      </c>
+      <c r="K8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B9" s="44" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C9">
+        <v>202412</v>
+      </c>
+      <c r="D9">
+        <v>164195594</v>
+      </c>
+      <c r="E9">
+        <v>59067147</v>
+      </c>
+      <c r="F9">
+        <v>166590275</v>
+      </c>
+      <c r="G9">
+        <v>61461828</v>
+      </c>
+      <c r="H9">
+        <v>10612172</v>
+      </c>
+      <c r="I9">
+        <v>-8217491</v>
+      </c>
+      <c r="J9">
+        <v>18829663</v>
+      </c>
+      <c r="K9">
+        <v>105128447</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="44" t="s">
         <v>1214</v>
       </c>
-      <c r="C9" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D9">
+      <c r="C10">
+        <v>202412</v>
+      </c>
+      <c r="D10">
+        <v>36755378</v>
+      </c>
+      <c r="E10">
+        <v>36755378</v>
+      </c>
+      <c r="F10">
+        <v>64791487</v>
+      </c>
+      <c r="G10">
+        <v>64791487</v>
+      </c>
+      <c r="H10">
+        <v>28036109</v>
+      </c>
+      <c r="I10">
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="J10">
+        <v>28036109</v>
+      </c>
+      <c r="K10">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B10" s="44" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="44" t="s">
         <v>852</v>
       </c>
-      <c r="C10" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D10">
-        <v>13276780</v>
-      </c>
-      <c r="E10">
-        <v>-77831635</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
-      <c r="B11" s="44"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>202412</v>
+      </c>
+      <c r="D11">
+        <v>1924958502</v>
+      </c>
+      <c r="E11">
+        <v>1293352057</v>
+      </c>
+      <c r="F11">
+        <v>1887250085</v>
+      </c>
+      <c r="G11">
+        <v>1255643640</v>
+      </c>
+      <c r="H11">
+        <v>-142440077</v>
+      </c>
+      <c r="I11">
+        <v>104731660</v>
+      </c>
+      <c r="J11">
+        <v>-247171737</v>
+      </c>
+      <c r="K11">
+        <v>631606445</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="44"/>
       <c r="B15" s="44"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
     </row>
@@ -55175,16 +55387,15 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A2B8D3-8697-8047-B90E-9EF188533867}">
-  <dimension ref="A1:K500"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E2F17F-B09D-944E-9EA4-A1F4C79AA9D1}">
+  <sheetPr codeName="Hoja6"/>
+  <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>1203</v>
       </c>
@@ -55195,397 +55406,186 @@
         <v>1229</v>
       </c>
       <c r="D1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="E1" t="s">
-        <v>1208</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1209</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1210</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1211</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1212</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1215</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>1074</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="C2">
-        <v>202412</v>
+      <c r="C2" s="45">
+        <v>45627</v>
       </c>
       <c r="D2">
-        <v>184648783</v>
+        <v>8824813</v>
       </c>
       <c r="E2">
-        <v>184648783</v>
-      </c>
-      <c r="F2">
-        <v>203895741</v>
-      </c>
-      <c r="G2">
-        <v>203895741</v>
-      </c>
-      <c r="H2">
-        <v>19246958</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>19246958</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-6875556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
         <v>1074</v>
       </c>
       <c r="B3" s="44" t="s">
         <v>839</v>
       </c>
-      <c r="C3">
-        <v>202412</v>
+      <c r="C3" s="45">
+        <v>45627</v>
       </c>
       <c r="D3">
-        <v>662347303</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>662347303</v>
-      </c>
-      <c r="F3">
-        <v>694786204</v>
-      </c>
-      <c r="G3">
-        <v>694786204</v>
-      </c>
-      <c r="H3">
-        <v>36305051</v>
-      </c>
-      <c r="I3">
-        <v>593</v>
-      </c>
-      <c r="J3">
-        <v>36304458</v>
-      </c>
-      <c r="K3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B4" s="44" t="s">
         <v>1075</v>
       </c>
-      <c r="C4">
-        <v>202412</v>
+      <c r="C4" s="45">
+        <v>45627</v>
       </c>
       <c r="D4">
-        <v>1427498894</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1427498894</v>
-      </c>
-      <c r="F4">
-        <v>1432785215</v>
-      </c>
-      <c r="G4">
-        <v>1432785215</v>
-      </c>
-      <c r="H4">
-        <v>5286321</v>
-      </c>
-      <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>5286321</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="C5">
-        <v>202412</v>
+      <c r="C5" s="45">
+        <v>45627</v>
       </c>
       <c r="D5">
-        <v>37620549295</v>
+        <v>574118578</v>
       </c>
       <c r="E5">
-        <v>34615671489</v>
-      </c>
-      <c r="F5">
-        <v>37727865277</v>
-      </c>
-      <c r="G5">
-        <v>34722987471</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>3004877806</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3878153423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B6" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="C6">
-        <v>202412</v>
+      <c r="C6" s="45">
+        <v>45627</v>
       </c>
       <c r="D6">
-        <v>179132945472</v>
+        <v>4952998587</v>
       </c>
       <c r="E6">
-        <v>179129728394</v>
-      </c>
-      <c r="F6">
-        <v>157701048874</v>
-      </c>
-      <c r="G6">
-        <v>157697831796</v>
-      </c>
-      <c r="H6">
-        <v>-21234067395</v>
-      </c>
-      <c r="I6">
-        <v>-197829203</v>
-      </c>
-      <c r="J6">
-        <v>-21036238192</v>
-      </c>
-      <c r="K6">
-        <v>3217078</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-4070914402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B7" s="44" t="s">
         <v>839</v>
       </c>
-      <c r="C7">
-        <v>202412</v>
+      <c r="C7" s="45">
+        <v>45627</v>
       </c>
       <c r="D7">
-        <v>4564533939</v>
+        <v>132659301</v>
       </c>
       <c r="E7">
-        <v>3488760438</v>
-      </c>
-      <c r="F7">
-        <v>4718335471</v>
-      </c>
-      <c r="G7">
-        <v>3642561970</v>
-      </c>
-      <c r="H7">
-        <v>429469879</v>
-      </c>
-      <c r="I7">
-        <v>-275668347</v>
-      </c>
-      <c r="J7">
-        <v>705138226</v>
-      </c>
-      <c r="K7">
-        <v>1075773501</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-134705661</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B8" s="44" t="s">
         <v>1077</v>
       </c>
-      <c r="C8">
-        <v>202412</v>
+      <c r="C8" s="45">
+        <v>45627</v>
       </c>
       <c r="D8">
-        <v>371614941</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>371614941</v>
-      </c>
-      <c r="F8">
-        <v>512133717</v>
-      </c>
-      <c r="G8">
-        <v>512133717</v>
-      </c>
-      <c r="H8">
-        <v>140518776</v>
-      </c>
-      <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>140518776</v>
-      </c>
-      <c r="K8">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C9" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C9">
-        <v>202412</v>
-      </c>
-      <c r="D9">
-        <v>164195594</v>
-      </c>
       <c r="E9">
-        <v>59067147</v>
-      </c>
-      <c r="F9">
-        <v>166590275</v>
-      </c>
-      <c r="G9">
-        <v>61461828</v>
-      </c>
-      <c r="H9">
-        <v>10612172</v>
-      </c>
-      <c r="I9">
-        <v>-8217491</v>
-      </c>
-      <c r="J9">
-        <v>18829663</v>
-      </c>
-      <c r="K9">
-        <v>105128447</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C10">
-        <v>202412</v>
+        <v>852</v>
+      </c>
+      <c r="C10" s="45">
+        <v>45627</v>
       </c>
       <c r="D10">
-        <v>36755378</v>
+        <v>13276780</v>
       </c>
       <c r="E10">
-        <v>36755378</v>
-      </c>
-      <c r="F10">
-        <v>64791487</v>
-      </c>
-      <c r="G10">
-        <v>64791487</v>
-      </c>
-      <c r="H10">
-        <v>28036109</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>28036109</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>852</v>
-      </c>
-      <c r="C11">
-        <v>202412</v>
-      </c>
-      <c r="D11">
-        <v>1924958502</v>
-      </c>
-      <c r="E11">
-        <v>1293352057</v>
-      </c>
-      <c r="F11">
-        <v>1887250085</v>
-      </c>
-      <c r="G11">
-        <v>1255643640</v>
-      </c>
-      <c r="H11">
-        <v>-142440077</v>
-      </c>
-      <c r="I11">
-        <v>104731660</v>
-      </c>
-      <c r="J11">
-        <v>-247171737</v>
-      </c>
-      <c r="K11">
-        <v>631606445</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-77831635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="44"/>
       <c r="B15" s="44"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
     </row>
@@ -57540,10 +57540,16 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57819,16 +57825,10 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57840,9 +57840,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
+    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -57868,19 +57878,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
-    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: Corregir formato de logs de la plantilla
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9DAD00-5E6F-2E41-972E-A631FCF651C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A49C7A-846C-2844-808D-8F236116989F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="22560" windowHeight="17380" tabRatio="844" firstSheet="3" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
@@ -21,8 +21,8 @@
     <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId7"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="21" r:id="rId8"/>
-    <sheet name="SAP_Sinis_Ced" sheetId="109" r:id="rId9"/>
-    <sheet name="add_p_SAP_Primas_Ced" sheetId="108" r:id="rId10"/>
+    <sheet name="add_p_SAP_Primas_Ced" sheetId="112" r:id="rId9"/>
+    <sheet name="SAP_Sinis_Ced" sheetId="109" r:id="rId10"/>
     <sheet name="add_p_Gastos_Expedicion" sheetId="18" r:id="rId11"/>
     <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId12"/>
   </sheets>
@@ -5574,15 +5574,15 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A129746-6CD1-624B-BD34-B413117965C4}">
-  <sheetPr codeName="Hoja7"/>
-  <dimension ref="A1:K500"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E2F17F-B09D-944E-9EA4-A1F4C79AA9D1}">
+  <sheetPr codeName="Hoja6"/>
+  <dimension ref="A1:E500"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>1203</v>
       </c>
@@ -5593,397 +5593,186 @@
         <v>1229</v>
       </c>
       <c r="D1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="E1" t="s">
-        <v>1208</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1209</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1210</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1211</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1212</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1215</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>1074</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="C2">
-        <v>202412</v>
+      <c r="C2" s="45">
+        <v>45627</v>
       </c>
       <c r="D2">
-        <v>184648783</v>
+        <v>8824813</v>
       </c>
       <c r="E2">
-        <v>184648783</v>
-      </c>
-      <c r="F2">
-        <v>203895741</v>
-      </c>
-      <c r="G2">
-        <v>203895741</v>
-      </c>
-      <c r="H2">
-        <v>19246958</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>19246958</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-6875556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
         <v>1074</v>
       </c>
       <c r="B3" s="44" t="s">
         <v>839</v>
       </c>
-      <c r="C3">
-        <v>202412</v>
+      <c r="C3" s="45">
+        <v>45627</v>
       </c>
       <c r="D3">
-        <v>662347303</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>662347303</v>
-      </c>
-      <c r="F3">
-        <v>694786204</v>
-      </c>
-      <c r="G3">
-        <v>694786204</v>
-      </c>
-      <c r="H3">
-        <v>36305051</v>
-      </c>
-      <c r="I3">
-        <v>593</v>
-      </c>
-      <c r="J3">
-        <v>36304458</v>
-      </c>
-      <c r="K3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B4" s="44" t="s">
         <v>1075</v>
       </c>
-      <c r="C4">
-        <v>202412</v>
+      <c r="C4" s="45">
+        <v>45627</v>
       </c>
       <c r="D4">
-        <v>1427498894</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1427498894</v>
-      </c>
-      <c r="F4">
-        <v>1432785215</v>
-      </c>
-      <c r="G4">
-        <v>1432785215</v>
-      </c>
-      <c r="H4">
-        <v>5286321</v>
-      </c>
-      <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>5286321</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="C5">
-        <v>202412</v>
+      <c r="C5" s="45">
+        <v>45627</v>
       </c>
       <c r="D5">
-        <v>37620549295</v>
+        <v>574118578</v>
       </c>
       <c r="E5">
-        <v>34615671489</v>
-      </c>
-      <c r="F5">
-        <v>37727865277</v>
-      </c>
-      <c r="G5">
-        <v>34722987471</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>3004877806</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3878153423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B6" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="C6">
-        <v>202412</v>
+      <c r="C6" s="45">
+        <v>45627</v>
       </c>
       <c r="D6">
-        <v>179132945472</v>
+        <v>4952998587</v>
       </c>
       <c r="E6">
-        <v>179129728394</v>
-      </c>
-      <c r="F6">
-        <v>157701048874</v>
-      </c>
-      <c r="G6">
-        <v>157697831796</v>
-      </c>
-      <c r="H6">
-        <v>-21234067395</v>
-      </c>
-      <c r="I6">
-        <v>-197829203</v>
-      </c>
-      <c r="J6">
-        <v>-21036238192</v>
-      </c>
-      <c r="K6">
-        <v>3217078</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-4070914402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B7" s="44" t="s">
         <v>839</v>
       </c>
-      <c r="C7">
-        <v>202412</v>
+      <c r="C7" s="45">
+        <v>45627</v>
       </c>
       <c r="D7">
-        <v>4564533939</v>
+        <v>132659301</v>
       </c>
       <c r="E7">
-        <v>3488760438</v>
-      </c>
-      <c r="F7">
-        <v>4718335471</v>
-      </c>
-      <c r="G7">
-        <v>3642561970</v>
-      </c>
-      <c r="H7">
-        <v>429469879</v>
-      </c>
-      <c r="I7">
-        <v>-275668347</v>
-      </c>
-      <c r="J7">
-        <v>705138226</v>
-      </c>
-      <c r="K7">
-        <v>1075773501</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-134705661</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B8" s="44" t="s">
         <v>1077</v>
       </c>
-      <c r="C8">
-        <v>202412</v>
+      <c r="C8" s="45">
+        <v>45627</v>
       </c>
       <c r="D8">
-        <v>371614941</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>371614941</v>
-      </c>
-      <c r="F8">
-        <v>512133717</v>
-      </c>
-      <c r="G8">
-        <v>512133717</v>
-      </c>
-      <c r="H8">
-        <v>140518776</v>
-      </c>
-      <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>140518776</v>
-      </c>
-      <c r="K8">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C9" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C9">
-        <v>202412</v>
-      </c>
-      <c r="D9">
-        <v>164195594</v>
-      </c>
       <c r="E9">
-        <v>59067147</v>
-      </c>
-      <c r="F9">
-        <v>166590275</v>
-      </c>
-      <c r="G9">
-        <v>61461828</v>
-      </c>
-      <c r="H9">
-        <v>10612172</v>
-      </c>
-      <c r="I9">
-        <v>-8217491</v>
-      </c>
-      <c r="J9">
-        <v>18829663</v>
-      </c>
-      <c r="K9">
-        <v>105128447</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C10">
-        <v>202412</v>
+        <v>852</v>
+      </c>
+      <c r="C10" s="45">
+        <v>45627</v>
       </c>
       <c r="D10">
-        <v>36755378</v>
+        <v>13276780</v>
       </c>
       <c r="E10">
-        <v>36755378</v>
-      </c>
-      <c r="F10">
-        <v>64791487</v>
-      </c>
-      <c r="G10">
-        <v>64791487</v>
-      </c>
-      <c r="H10">
-        <v>28036109</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>28036109</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>852</v>
-      </c>
-      <c r="C11">
-        <v>202412</v>
-      </c>
-      <c r="D11">
-        <v>1924958502</v>
-      </c>
-      <c r="E11">
-        <v>1293352057</v>
-      </c>
-      <c r="F11">
-        <v>1887250085</v>
-      </c>
-      <c r="G11">
-        <v>1255643640</v>
-      </c>
-      <c r="H11">
-        <v>-142440077</v>
-      </c>
-      <c r="I11">
-        <v>104731660</v>
-      </c>
-      <c r="J11">
-        <v>-247171737</v>
-      </c>
-      <c r="K11">
-        <v>631606445</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-77831635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="44"/>
       <c r="B15" s="44"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
     </row>
@@ -55387,15 +55176,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E2F17F-B09D-944E-9EA4-A1F4C79AA9D1}">
-  <sheetPr codeName="Hoja6"/>
-  <dimension ref="A1:E500"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3B42F4-1841-984B-BE93-9807147BD0DF}">
+  <dimension ref="A1:K500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>1203</v>
       </c>
@@ -55406,186 +55194,397 @@
         <v>1229</v>
       </c>
       <c r="D1" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
       <c r="E1" t="s">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1208</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>1074</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="45">
-        <v>45627</v>
+      <c r="C2">
+        <v>202501</v>
       </c>
       <c r="D2">
-        <v>8824813</v>
+        <v>173399188</v>
       </c>
       <c r="E2">
-        <v>-6875556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>173399188</v>
+      </c>
+      <c r="F2">
+        <v>210675369</v>
+      </c>
+      <c r="G2">
+        <v>210675369</v>
+      </c>
+      <c r="H2">
+        <v>22320594</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>22320594</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
         <v>1074</v>
       </c>
       <c r="B3" s="44" t="s">
         <v>839</v>
       </c>
-      <c r="C3" s="45">
-        <v>45627</v>
+      <c r="C3">
+        <v>202501</v>
       </c>
       <c r="D3">
+        <v>436803319</v>
+      </c>
+      <c r="E3">
+        <v>436803319</v>
+      </c>
+      <c r="F3">
+        <v>512257135</v>
+      </c>
+      <c r="G3">
+        <v>512257135</v>
+      </c>
+      <c r="H3">
+        <v>69015494</v>
+      </c>
+      <c r="I3">
+        <v>-6</v>
+      </c>
+      <c r="J3">
+        <v>69015500</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B4" s="44" t="s">
         <v>1075</v>
       </c>
-      <c r="C4" s="45">
-        <v>45627</v>
+      <c r="C4">
+        <v>202501</v>
       </c>
       <c r="D4">
+        <v>1308582154</v>
+      </c>
+      <c r="E4">
+        <v>1308582154</v>
+      </c>
+      <c r="F4">
+        <v>1341478541</v>
+      </c>
+      <c r="G4">
+        <v>1341478541</v>
+      </c>
+      <c r="H4">
+        <v>32896387</v>
+      </c>
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="J4">
+        <v>32896387</v>
+      </c>
+      <c r="K4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="45">
-        <v>45627</v>
+      <c r="C5">
+        <v>202501</v>
       </c>
       <c r="D5">
-        <v>574118578</v>
+        <v>32448805638</v>
       </c>
       <c r="E5">
-        <v>3878153423</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>30676649972</v>
+      </c>
+      <c r="F5">
+        <v>39334196918</v>
+      </c>
+      <c r="G5">
+        <v>37562041252</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1772155666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B6" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="45">
-        <v>45627</v>
+      <c r="C6">
+        <v>202501</v>
       </c>
       <c r="D6">
-        <v>4952998587</v>
+        <v>47590494159</v>
       </c>
       <c r="E6">
-        <v>-4070914402</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>45361868519</v>
+      </c>
+      <c r="F6">
+        <v>72082837725</v>
+      </c>
+      <c r="G6">
+        <v>69854212085</v>
+      </c>
+      <c r="H6">
+        <v>22477822788</v>
+      </c>
+      <c r="I6">
+        <v>2014520778</v>
+      </c>
+      <c r="J6">
+        <v>20463302010</v>
+      </c>
+      <c r="K6">
+        <v>2228625640</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B7" s="44" t="s">
         <v>839</v>
       </c>
-      <c r="C7" s="45">
-        <v>45627</v>
+      <c r="C7">
+        <v>202501</v>
       </c>
       <c r="D7">
-        <v>132659301</v>
+        <v>5400889117</v>
       </c>
       <c r="E7">
-        <v>-134705661</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3407840127</v>
+      </c>
+      <c r="F7">
+        <v>5385171178</v>
+      </c>
+      <c r="G7">
+        <v>3392122188</v>
+      </c>
+      <c r="H7">
+        <v>-674093825</v>
+      </c>
+      <c r="I7">
+        <v>658375886</v>
+      </c>
+      <c r="J7">
+        <v>-1332469711</v>
+      </c>
+      <c r="K7">
+        <v>1993048990</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B8" s="44" t="s">
         <v>1077</v>
       </c>
-      <c r="C8" s="45">
-        <v>45627</v>
+      <c r="C8">
+        <v>202501</v>
       </c>
       <c r="D8">
+        <v>303769141</v>
+      </c>
+      <c r="E8">
+        <v>303769141</v>
+      </c>
+      <c r="F8">
+        <v>492130820</v>
+      </c>
+      <c r="G8">
+        <v>492130820</v>
+      </c>
+      <c r="H8">
+        <v>188361679</v>
+      </c>
+      <c r="I8">
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="J8">
+        <v>188361679</v>
+      </c>
+      <c r="K8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="44" t="s">
         <v>148</v>
       </c>
       <c r="B9" s="44" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C9">
+        <v>202501</v>
+      </c>
+      <c r="D9">
+        <v>158252436</v>
+      </c>
+      <c r="E9">
+        <v>57071142</v>
+      </c>
+      <c r="F9">
+        <v>158748472</v>
+      </c>
+      <c r="G9">
+        <v>57567178</v>
+      </c>
+      <c r="H9">
+        <v>2469611</v>
+      </c>
+      <c r="I9">
+        <v>-1973575</v>
+      </c>
+      <c r="J9">
+        <v>4443186</v>
+      </c>
+      <c r="K9">
+        <v>101181294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="44" t="s">
         <v>1214</v>
       </c>
-      <c r="C9" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D9">
+      <c r="C10">
+        <v>202501</v>
+      </c>
+      <c r="D10">
+        <v>53021962</v>
+      </c>
+      <c r="E10">
+        <v>53021962</v>
+      </c>
+      <c r="F10">
+        <v>66253328</v>
+      </c>
+      <c r="G10">
+        <v>66253328</v>
+      </c>
+      <c r="H10">
+        <v>13231366</v>
+      </c>
+      <c r="I10">
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="J10">
+        <v>13231366</v>
+      </c>
+      <c r="K10">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B10" s="44" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="44" t="s">
         <v>852</v>
       </c>
-      <c r="C10" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D10">
-        <v>13276780</v>
-      </c>
-      <c r="E10">
-        <v>-77831635</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
-      <c r="B11" s="44"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>202501</v>
+      </c>
+      <c r="D11">
+        <v>1123643875</v>
+      </c>
+      <c r="E11">
+        <v>764972652</v>
+      </c>
+      <c r="F11">
+        <v>1422300938</v>
+      </c>
+      <c r="G11">
+        <v>1063629715</v>
+      </c>
+      <c r="H11">
+        <v>465607073</v>
+      </c>
+      <c r="I11">
+        <v>-166950010</v>
+      </c>
+      <c r="J11">
+        <v>632557083</v>
+      </c>
+      <c r="K11">
+        <v>358671223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="44"/>
       <c r="B15" s="44"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
     </row>
@@ -57531,28 +57530,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F504A30D0A8B7C48AC3312637B06038A" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18aa81df5b435925a4ef391b68c25b4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="df0aad82-cca9-4ab3-a26b-b2d93ab652bf" xmlns:ns3="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019c64929386a1d9ec4afd0363aaee9d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -57824,40 +57808,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
-    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -57877,10 +57858,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
+    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Definir aperturas para cuadre contable desde el Excel
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A49C7A-846C-2844-808D-8F236116989F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0B69B1-95F4-BA4F-B01F-B7FA6A413EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22560" windowHeight="17380" tabRatio="844" firstSheet="3" activeTab="8" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22560" windowHeight="17380" tabRatio="844" firstSheet="3" activeTab="6" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="add_pe_Canal-Poliza" sheetId="8" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="add_e_Amparos" sheetId="1" r:id="rId4"/>
     <sheet name="Atipicos" sheetId="14" r:id="rId5"/>
     <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId6"/>
-    <sheet name="Cuadre_Contable_Siniestros" sheetId="20" r:id="rId7"/>
-    <sheet name="Cuadre_Contable_Primas" sheetId="21" r:id="rId8"/>
+    <sheet name="Cuadre_Siniestros" sheetId="20" r:id="rId7"/>
+    <sheet name="Cuadre_Primas" sheetId="21" r:id="rId8"/>
     <sheet name="add_p_SAP_Primas_Ced" sheetId="112" r:id="rId9"/>
     <sheet name="SAP_Sinis_Ced" sheetId="109" r:id="rId10"/>
     <sheet name="add_p_Gastos_Expedicion" sheetId="18" r:id="rId11"/>
@@ -54536,9 +54536,7 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -55179,7 +55177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3B42F4-1841-984B-BE93-9807147BD0DF}">
   <dimension ref="A1:K500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -57530,10 +57528,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57809,16 +57813,10 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57831,9 +57829,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
+    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -57859,19 +57867,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b"/>
-    <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Establecer query consolidado de siniestros de autonomia como metodo principal de extraccion, dejando el metodo de Polars como fallback
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,34 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615E1941-01CF-2240-AB87-EE76C654C1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F926EA-2F2C-7C44-9197-CF06657FFAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30380" yWindow="640" windowWidth="38080" windowHeight="20780" tabRatio="844" activeTab="2" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" tabRatio="844" firstSheet="5" activeTab="11" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Aperturas_Siniestros" sheetId="113" r:id="rId1"/>
     <sheet name="Aperturas_Primas" sheetId="115" r:id="rId2"/>
     <sheet name="Aperturas_Expuestos" sheetId="114" r:id="rId3"/>
-    <sheet name="add_pe_Canal-Poliza" sheetId="8" r:id="rId4"/>
-    <sheet name="add_pe_Canal-Canal" sheetId="12" r:id="rId5"/>
-    <sheet name="add_pe_Canal-Sucursal" sheetId="9" r:id="rId6"/>
-    <sheet name="add_e_Amparos" sheetId="1" r:id="rId7"/>
-    <sheet name="Atipicos" sheetId="14" r:id="rId8"/>
-    <sheet name="Inc_Ced_Atipicos" sheetId="17" r:id="rId9"/>
+    <sheet name="add_spe_Canal-Poliza" sheetId="8" r:id="rId4"/>
+    <sheet name="add_spe_Canal-Canal" sheetId="12" r:id="rId5"/>
+    <sheet name="add_spe_Canal-Sucursal" sheetId="9" r:id="rId6"/>
+    <sheet name="add_se_Amparos" sheetId="1" r:id="rId7"/>
+    <sheet name="add_s_Atipicos" sheetId="14" r:id="rId8"/>
+    <sheet name="add_s_Inc_Ced_Atipicos" sheetId="17" r:id="rId9"/>
     <sheet name="Cuadre_Siniestros" sheetId="20" r:id="rId10"/>
     <sheet name="Cuadre_Primas" sheetId="21" r:id="rId11"/>
-    <sheet name="add_p_SAP_Primas_Ced" sheetId="112" r:id="rId12"/>
-    <sheet name="SAP_Sinis_Ced" sheetId="109" r:id="rId13"/>
+    <sheet name="add_s_SAP_Sinis_Ced" sheetId="109" r:id="rId12"/>
+    <sheet name="add_p_SAP_Primas_Ced" sheetId="112" r:id="rId13"/>
     <sheet name="add_p_Gastos_Expedicion" sheetId="18" r:id="rId14"/>
     <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">add_e_Amparos!$A$1:$G$230</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'add_pe_Canal-Poliza'!$B$1:$G$43</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'add_pe_Canal-Sucursal'!$C$1:$G$2126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">add_s_Atipicos!$A$1:$G$1063</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">add_s_Inc_Ced_Atipicos!$A$1:$M$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">add_se_Amparos!$A$1:$G$230</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'add_spe_Canal-Poliza'!$B$1:$G$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'add_spe_Canal-Sucursal'!$C$1:$G$2126</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Amparos_Negocio_083!$A$1:$B$80</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Atipicos!$A$1:$G$1063</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Inc_Ced_Atipicos!$A$1:$M$29</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -6235,6 +6235,2152 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E2F17F-B09D-944E-9EA4-A1F4C79AA9D1}">
+  <sheetPr codeName="Hoja6"/>
+  <dimension ref="A1:E500"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="44" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="44" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D2">
+        <v>8824813</v>
+      </c>
+      <c r="E2">
+        <v>-6875556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="44" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>839</v>
+      </c>
+      <c r="C3" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C4" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D5">
+        <v>574118578</v>
+      </c>
+      <c r="E5">
+        <v>3878153423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D6">
+        <v>4952998587</v>
+      </c>
+      <c r="E6">
+        <v>-4070914402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>839</v>
+      </c>
+      <c r="C7" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D7">
+        <v>132659301</v>
+      </c>
+      <c r="E7">
+        <v>-134705661</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C8" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C9" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>852</v>
+      </c>
+      <c r="C10" s="45">
+        <v>45627</v>
+      </c>
+      <c r="D10">
+        <v>13276780</v>
+      </c>
+      <c r="E10">
+        <v>-77831635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="44"/>
+      <c r="B28" s="44"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="44"/>
+      <c r="B30" s="44"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="44"/>
+      <c r="B32" s="44"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="44"/>
+      <c r="B33" s="44"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="44"/>
+      <c r="B36" s="44"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="44"/>
+      <c r="B37" s="44"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="44"/>
+      <c r="B38" s="44"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="44"/>
+      <c r="B39" s="44"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="44"/>
+      <c r="B41" s="44"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="44"/>
+      <c r="B45" s="44"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="44"/>
+      <c r="B47" s="44"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="44"/>
+      <c r="B48" s="44"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="44"/>
+      <c r="B49" s="44"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="44"/>
+      <c r="B50" s="44"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="44"/>
+      <c r="B51" s="44"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="44"/>
+      <c r="B52" s="44"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="44"/>
+      <c r="B53" s="44"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="44"/>
+      <c r="B54" s="44"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="44"/>
+      <c r="B55" s="44"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="44"/>
+      <c r="B57" s="44"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="44"/>
+      <c r="B58" s="44"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="44"/>
+      <c r="B59" s="44"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="44"/>
+      <c r="B60" s="44"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="44"/>
+      <c r="B61" s="44"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="44"/>
+      <c r="B62" s="44"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="44"/>
+      <c r="B63" s="44"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="44"/>
+      <c r="B64" s="44"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="44"/>
+      <c r="B65" s="44"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="44"/>
+      <c r="B66" s="44"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="44"/>
+      <c r="B67" s="44"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="44"/>
+      <c r="B68" s="44"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="44"/>
+      <c r="B69" s="44"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="44"/>
+      <c r="B70" s="44"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="44"/>
+      <c r="B71" s="44"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="44"/>
+      <c r="B72" s="44"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="44"/>
+      <c r="B73" s="44"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="44"/>
+      <c r="B74" s="44"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="44"/>
+      <c r="B75" s="44"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="44"/>
+      <c r="B76" s="44"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="44"/>
+      <c r="B77" s="44"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="44"/>
+      <c r="B78" s="44"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="44"/>
+      <c r="B79" s="44"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="44"/>
+      <c r="B80" s="44"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="44"/>
+      <c r="B81" s="44"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="44"/>
+      <c r="B82" s="44"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="44"/>
+      <c r="B86" s="44"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="44"/>
+      <c r="B88" s="44"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="44"/>
+      <c r="B89" s="44"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="44"/>
+      <c r="B90" s="44"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="44"/>
+      <c r="B91" s="44"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="44"/>
+      <c r="B92" s="44"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="44"/>
+      <c r="B93" s="44"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="44"/>
+      <c r="B94" s="44"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="44"/>
+      <c r="B95" s="44"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="44"/>
+      <c r="B96" s="44"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="44"/>
+      <c r="B97" s="44"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="44"/>
+      <c r="B98" s="44"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="44"/>
+      <c r="B99" s="44"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="44"/>
+      <c r="B100" s="44"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="44"/>
+      <c r="B101" s="44"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="44"/>
+      <c r="B102" s="44"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="44"/>
+      <c r="B103" s="44"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="44"/>
+      <c r="B104" s="44"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="44"/>
+      <c r="B105" s="44"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="44"/>
+      <c r="B106" s="44"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="44"/>
+      <c r="B107" s="44"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="44"/>
+      <c r="B108" s="44"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="44"/>
+      <c r="B109" s="44"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="44"/>
+      <c r="B110" s="44"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="44"/>
+      <c r="B111" s="44"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="44"/>
+      <c r="B112" s="44"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="44"/>
+      <c r="B113" s="44"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="44"/>
+      <c r="B114" s="44"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="44"/>
+      <c r="B115" s="44"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="44"/>
+      <c r="B116" s="44"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="44"/>
+      <c r="B117" s="44"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="44"/>
+      <c r="B118" s="44"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="44"/>
+      <c r="B119" s="44"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="44"/>
+      <c r="B120" s="44"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="44"/>
+      <c r="B121" s="44"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="44"/>
+      <c r="B122" s="44"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="44"/>
+      <c r="B123" s="44"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="44"/>
+      <c r="B124" s="44"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="44"/>
+      <c r="B125" s="44"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="44"/>
+      <c r="B126" s="44"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="44"/>
+      <c r="B127" s="44"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="44"/>
+      <c r="B128" s="44"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="44"/>
+      <c r="B129" s="44"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="44"/>
+      <c r="B130" s="44"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="44"/>
+      <c r="B131" s="44"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="44"/>
+      <c r="B132" s="44"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="44"/>
+      <c r="B133" s="44"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="44"/>
+      <c r="B134" s="44"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="44"/>
+      <c r="B135" s="44"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="44"/>
+      <c r="B136" s="44"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="44"/>
+      <c r="B137" s="44"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="44"/>
+      <c r="B138" s="44"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="44"/>
+      <c r="B139" s="44"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="44"/>
+      <c r="B140" s="44"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="44"/>
+      <c r="B141" s="44"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="44"/>
+      <c r="B142" s="44"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="44"/>
+      <c r="B143" s="44"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="44"/>
+      <c r="B144" s="44"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="44"/>
+      <c r="B145" s="44"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="44"/>
+      <c r="B146" s="44"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="44"/>
+      <c r="B147" s="44"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="44"/>
+      <c r="B148" s="44"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="44"/>
+      <c r="B149" s="44"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="44"/>
+      <c r="B150" s="44"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="44"/>
+      <c r="B151" s="44"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="44"/>
+      <c r="B152" s="44"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="44"/>
+      <c r="B153" s="44"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="44"/>
+      <c r="B154" s="44"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="44"/>
+      <c r="B155" s="44"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="44"/>
+      <c r="B156" s="44"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="44"/>
+      <c r="B157" s="44"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="44"/>
+      <c r="B158" s="44"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="44"/>
+      <c r="B159" s="44"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="44"/>
+      <c r="B160" s="44"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="44"/>
+      <c r="B161" s="44"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="44"/>
+      <c r="B162" s="44"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="44"/>
+      <c r="B163" s="44"/>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="44"/>
+      <c r="B164" s="44"/>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="44"/>
+      <c r="B165" s="44"/>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="44"/>
+      <c r="B166" s="44"/>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="44"/>
+      <c r="B167" s="44"/>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="44"/>
+      <c r="B168" s="44"/>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="44"/>
+      <c r="B169" s="44"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="44"/>
+      <c r="B170" s="44"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="44"/>
+      <c r="B171" s="44"/>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="44"/>
+      <c r="B172" s="44"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="44"/>
+      <c r="B173" s="44"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="44"/>
+      <c r="B174" s="44"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="44"/>
+      <c r="B175" s="44"/>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="44"/>
+      <c r="B176" s="44"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="44"/>
+      <c r="B177" s="44"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="44"/>
+      <c r="B178" s="44"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="44"/>
+      <c r="B179" s="44"/>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="44"/>
+      <c r="B180" s="44"/>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="44"/>
+      <c r="B181" s="44"/>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="44"/>
+      <c r="B182" s="44"/>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="44"/>
+      <c r="B183" s="44"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="44"/>
+      <c r="B184" s="44"/>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="44"/>
+      <c r="B185" s="44"/>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="44"/>
+      <c r="B186" s="44"/>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="44"/>
+      <c r="B187" s="44"/>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="44"/>
+      <c r="B188" s="44"/>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="44"/>
+      <c r="B189" s="44"/>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="44"/>
+      <c r="B190" s="44"/>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="44"/>
+      <c r="B191" s="44"/>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="44"/>
+      <c r="B192" s="44"/>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="44"/>
+      <c r="B193" s="44"/>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="44"/>
+      <c r="B194" s="44"/>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="44"/>
+      <c r="B195" s="44"/>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="44"/>
+      <c r="B196" s="44"/>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="44"/>
+      <c r="B197" s="44"/>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="44"/>
+      <c r="B198" s="44"/>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="44"/>
+      <c r="B199" s="44"/>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="44"/>
+      <c r="B200" s="44"/>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="44"/>
+      <c r="B201" s="44"/>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="44"/>
+      <c r="B202" s="44"/>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="44"/>
+      <c r="B203" s="44"/>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="44"/>
+      <c r="B204" s="44"/>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="44"/>
+      <c r="B205" s="44"/>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="44"/>
+      <c r="B206" s="44"/>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="44"/>
+      <c r="B207" s="44"/>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="44"/>
+      <c r="B208" s="44"/>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="44"/>
+      <c r="B209" s="44"/>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="44"/>
+      <c r="B210" s="44"/>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="44"/>
+      <c r="B211" s="44"/>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="44"/>
+      <c r="B212" s="44"/>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="44"/>
+      <c r="B213" s="44"/>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="44"/>
+      <c r="B214" s="44"/>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="44"/>
+      <c r="B215" s="44"/>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="44"/>
+      <c r="B216" s="44"/>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="44"/>
+      <c r="B217" s="44"/>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="44"/>
+      <c r="B218" s="44"/>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="44"/>
+      <c r="B219" s="44"/>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="44"/>
+      <c r="B220" s="44"/>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="44"/>
+      <c r="B221" s="44"/>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="44"/>
+      <c r="B222" s="44"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="44"/>
+      <c r="B223" s="44"/>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="44"/>
+      <c r="B224" s="44"/>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="44"/>
+      <c r="B225" s="44"/>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="44"/>
+      <c r="B226" s="44"/>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="44"/>
+      <c r="B227" s="44"/>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="44"/>
+      <c r="B228" s="44"/>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="44"/>
+      <c r="B229" s="44"/>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="44"/>
+      <c r="B230" s="44"/>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="44"/>
+      <c r="B231" s="44"/>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="44"/>
+      <c r="B232" s="44"/>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="44"/>
+      <c r="B233" s="44"/>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="44"/>
+      <c r="B234" s="44"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" s="44"/>
+      <c r="B235" s="44"/>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="44"/>
+      <c r="B236" s="44"/>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="44"/>
+      <c r="B237" s="44"/>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="44"/>
+      <c r="B238" s="44"/>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="44"/>
+      <c r="B239" s="44"/>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="44"/>
+      <c r="B240" s="44"/>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="44"/>
+      <c r="B241" s="44"/>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="44"/>
+      <c r="B242" s="44"/>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" s="44"/>
+      <c r="B243" s="44"/>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="44"/>
+      <c r="B244" s="44"/>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="44"/>
+      <c r="B245" s="44"/>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" s="44"/>
+      <c r="B246" s="44"/>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="44"/>
+      <c r="B247" s="44"/>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="44"/>
+      <c r="B248" s="44"/>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="44"/>
+      <c r="B249" s="44"/>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="44"/>
+      <c r="B250" s="44"/>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" s="44"/>
+      <c r="B251" s="44"/>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" s="44"/>
+      <c r="B252" s="44"/>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" s="44"/>
+      <c r="B253" s="44"/>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" s="44"/>
+      <c r="B254" s="44"/>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" s="44"/>
+      <c r="B255" s="44"/>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" s="44"/>
+      <c r="B256" s="44"/>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257" s="44"/>
+      <c r="B257" s="44"/>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258" s="44"/>
+      <c r="B258" s="44"/>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259" s="44"/>
+      <c r="B259" s="44"/>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260" s="44"/>
+      <c r="B260" s="44"/>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" s="44"/>
+      <c r="B261" s="44"/>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" s="44"/>
+      <c r="B262" s="44"/>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263" s="44"/>
+      <c r="B263" s="44"/>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264" s="44"/>
+      <c r="B264" s="44"/>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" s="44"/>
+      <c r="B265" s="44"/>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" s="44"/>
+      <c r="B266" s="44"/>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267" s="44"/>
+      <c r="B267" s="44"/>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268" s="44"/>
+      <c r="B268" s="44"/>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269" s="44"/>
+      <c r="B269" s="44"/>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270" s="44"/>
+      <c r="B270" s="44"/>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" s="44"/>
+      <c r="B271" s="44"/>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272" s="44"/>
+      <c r="B272" s="44"/>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273" s="44"/>
+      <c r="B273" s="44"/>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" s="44"/>
+      <c r="B274" s="44"/>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275" s="44"/>
+      <c r="B275" s="44"/>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" s="44"/>
+      <c r="B276" s="44"/>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" s="44"/>
+      <c r="B277" s="44"/>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" s="44"/>
+      <c r="B278" s="44"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="44"/>
+      <c r="B279" s="44"/>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="44"/>
+      <c r="B280" s="44"/>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="44"/>
+      <c r="B281" s="44"/>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="44"/>
+      <c r="B282" s="44"/>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" s="44"/>
+      <c r="B283" s="44"/>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="44"/>
+      <c r="B284" s="44"/>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" s="44"/>
+      <c r="B285" s="44"/>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286" s="44"/>
+      <c r="B286" s="44"/>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" s="44"/>
+      <c r="B287" s="44"/>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288" s="44"/>
+      <c r="B288" s="44"/>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A289" s="44"/>
+      <c r="B289" s="44"/>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" s="44"/>
+      <c r="B290" s="44"/>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A291" s="44"/>
+      <c r="B291" s="44"/>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A292" s="44"/>
+      <c r="B292" s="44"/>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A293" s="44"/>
+      <c r="B293" s="44"/>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A294" s="44"/>
+      <c r="B294" s="44"/>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A295" s="44"/>
+      <c r="B295" s="44"/>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A296" s="44"/>
+      <c r="B296" s="44"/>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A297" s="44"/>
+      <c r="B297" s="44"/>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A298" s="44"/>
+      <c r="B298" s="44"/>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A299" s="44"/>
+      <c r="B299" s="44"/>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A300" s="44"/>
+      <c r="B300" s="44"/>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A301" s="44"/>
+      <c r="B301" s="44"/>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A302" s="44"/>
+      <c r="B302" s="44"/>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A303" s="44"/>
+      <c r="B303" s="44"/>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A304" s="44"/>
+      <c r="B304" s="44"/>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A305" s="44"/>
+      <c r="B305" s="44"/>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A306" s="44"/>
+      <c r="B306" s="44"/>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A307" s="44"/>
+      <c r="B307" s="44"/>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A308" s="44"/>
+      <c r="B308" s="44"/>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A309" s="44"/>
+      <c r="B309" s="44"/>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A310" s="44"/>
+      <c r="B310" s="44"/>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A311" s="44"/>
+      <c r="B311" s="44"/>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A312" s="44"/>
+      <c r="B312" s="44"/>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A313" s="44"/>
+      <c r="B313" s="44"/>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A314" s="44"/>
+      <c r="B314" s="44"/>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A315" s="44"/>
+      <c r="B315" s="44"/>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A316" s="44"/>
+      <c r="B316" s="44"/>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A317" s="44"/>
+      <c r="B317" s="44"/>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A318" s="44"/>
+      <c r="B318" s="44"/>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A319" s="44"/>
+      <c r="B319" s="44"/>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A320" s="44"/>
+      <c r="B320" s="44"/>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" s="44"/>
+      <c r="B321" s="44"/>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" s="44"/>
+      <c r="B322" s="44"/>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A323" s="44"/>
+      <c r="B323" s="44"/>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A324" s="44"/>
+      <c r="B324" s="44"/>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A325" s="44"/>
+      <c r="B325" s="44"/>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A326" s="44"/>
+      <c r="B326" s="44"/>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A327" s="44"/>
+      <c r="B327" s="44"/>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A328" s="44"/>
+      <c r="B328" s="44"/>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A329" s="44"/>
+      <c r="B329" s="44"/>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A330" s="44"/>
+      <c r="B330" s="44"/>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A331" s="44"/>
+      <c r="B331" s="44"/>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A332" s="44"/>
+      <c r="B332" s="44"/>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A333" s="44"/>
+      <c r="B333" s="44"/>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A334" s="44"/>
+      <c r="B334" s="44"/>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A335" s="44"/>
+      <c r="B335" s="44"/>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A336" s="44"/>
+      <c r="B336" s="44"/>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A337" s="44"/>
+      <c r="B337" s="44"/>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A338" s="44"/>
+      <c r="B338" s="44"/>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A339" s="44"/>
+      <c r="B339" s="44"/>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A340" s="44"/>
+      <c r="B340" s="44"/>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A341" s="44"/>
+      <c r="B341" s="44"/>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A342" s="44"/>
+      <c r="B342" s="44"/>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A343" s="44"/>
+      <c r="B343" s="44"/>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A344" s="44"/>
+      <c r="B344" s="44"/>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A345" s="44"/>
+      <c r="B345" s="44"/>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A346" s="44"/>
+      <c r="B346" s="44"/>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A347" s="44"/>
+      <c r="B347" s="44"/>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A348" s="44"/>
+      <c r="B348" s="44"/>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A349" s="44"/>
+      <c r="B349" s="44"/>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A350" s="44"/>
+      <c r="B350" s="44"/>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A351" s="44"/>
+      <c r="B351" s="44"/>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A352" s="44"/>
+      <c r="B352" s="44"/>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A353" s="44"/>
+      <c r="B353" s="44"/>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A354" s="44"/>
+      <c r="B354" s="44"/>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A355" s="44"/>
+      <c r="B355" s="44"/>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A356" s="44"/>
+      <c r="B356" s="44"/>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A357" s="44"/>
+      <c r="B357" s="44"/>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A358" s="44"/>
+      <c r="B358" s="44"/>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A359" s="44"/>
+      <c r="B359" s="44"/>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A360" s="44"/>
+      <c r="B360" s="44"/>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A361" s="44"/>
+      <c r="B361" s="44"/>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A362" s="44"/>
+      <c r="B362" s="44"/>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A363" s="44"/>
+      <c r="B363" s="44"/>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A364" s="44"/>
+      <c r="B364" s="44"/>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A365" s="44"/>
+      <c r="B365" s="44"/>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A366" s="44"/>
+      <c r="B366" s="44"/>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A367" s="44"/>
+      <c r="B367" s="44"/>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A368" s="44"/>
+      <c r="B368" s="44"/>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A369" s="44"/>
+      <c r="B369" s="44"/>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A370" s="44"/>
+      <c r="B370" s="44"/>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A371" s="44"/>
+      <c r="B371" s="44"/>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A372" s="44"/>
+      <c r="B372" s="44"/>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A373" s="44"/>
+      <c r="B373" s="44"/>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A374" s="44"/>
+      <c r="B374" s="44"/>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A375" s="44"/>
+      <c r="B375" s="44"/>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A376" s="44"/>
+      <c r="B376" s="44"/>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A377" s="44"/>
+      <c r="B377" s="44"/>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A378" s="44"/>
+      <c r="B378" s="44"/>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A379" s="44"/>
+      <c r="B379" s="44"/>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A380" s="44"/>
+      <c r="B380" s="44"/>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A381" s="44"/>
+      <c r="B381" s="44"/>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A382" s="44"/>
+      <c r="B382" s="44"/>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A383" s="44"/>
+      <c r="B383" s="44"/>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A384" s="44"/>
+      <c r="B384" s="44"/>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A385" s="44"/>
+      <c r="B385" s="44"/>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A386" s="44"/>
+      <c r="B386" s="44"/>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A387" s="44"/>
+      <c r="B387" s="44"/>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A388" s="44"/>
+      <c r="B388" s="44"/>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A389" s="44"/>
+      <c r="B389" s="44"/>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A390" s="44"/>
+      <c r="B390" s="44"/>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A391" s="44"/>
+      <c r="B391" s="44"/>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A392" s="44"/>
+      <c r="B392" s="44"/>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A393" s="44"/>
+      <c r="B393" s="44"/>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A394" s="44"/>
+      <c r="B394" s="44"/>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A395" s="44"/>
+      <c r="B395" s="44"/>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A396" s="44"/>
+      <c r="B396" s="44"/>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A397" s="44"/>
+      <c r="B397" s="44"/>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A398" s="44"/>
+      <c r="B398" s="44"/>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A399" s="44"/>
+      <c r="B399" s="44"/>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A400" s="44"/>
+      <c r="B400" s="44"/>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A401" s="44"/>
+      <c r="B401" s="44"/>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A402" s="44"/>
+      <c r="B402" s="44"/>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A403" s="44"/>
+      <c r="B403" s="44"/>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A404" s="44"/>
+      <c r="B404" s="44"/>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A405" s="44"/>
+      <c r="B405" s="44"/>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A406" s="44"/>
+      <c r="B406" s="44"/>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A407" s="44"/>
+      <c r="B407" s="44"/>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A408" s="44"/>
+      <c r="B408" s="44"/>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A409" s="44"/>
+      <c r="B409" s="44"/>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A410" s="44"/>
+      <c r="B410" s="44"/>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A411" s="44"/>
+      <c r="B411" s="44"/>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A412" s="44"/>
+      <c r="B412" s="44"/>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A413" s="44"/>
+      <c r="B413" s="44"/>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A414" s="44"/>
+      <c r="B414" s="44"/>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A415" s="44"/>
+      <c r="B415" s="44"/>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A416" s="44"/>
+      <c r="B416" s="44"/>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A417" s="44"/>
+      <c r="B417" s="44"/>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A418" s="44"/>
+      <c r="B418" s="44"/>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A419" s="44"/>
+      <c r="B419" s="44"/>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A420" s="44"/>
+      <c r="B420" s="44"/>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A421" s="44"/>
+      <c r="B421" s="44"/>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A422" s="44"/>
+      <c r="B422" s="44"/>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A423" s="44"/>
+      <c r="B423" s="44"/>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A424" s="44"/>
+      <c r="B424" s="44"/>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A425" s="44"/>
+      <c r="B425" s="44"/>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A426" s="44"/>
+      <c r="B426" s="44"/>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A427" s="44"/>
+      <c r="B427" s="44"/>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A428" s="44"/>
+      <c r="B428" s="44"/>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A429" s="44"/>
+      <c r="B429" s="44"/>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A430" s="44"/>
+      <c r="B430" s="44"/>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A431" s="44"/>
+      <c r="B431" s="44"/>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A432" s="44"/>
+      <c r="B432" s="44"/>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A433" s="44"/>
+      <c r="B433" s="44"/>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A434" s="44"/>
+      <c r="B434" s="44"/>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A435" s="44"/>
+      <c r="B435" s="44"/>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A436" s="44"/>
+      <c r="B436" s="44"/>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A437" s="44"/>
+      <c r="B437" s="44"/>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A438" s="44"/>
+      <c r="B438" s="44"/>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A439" s="44"/>
+      <c r="B439" s="44"/>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A440" s="44"/>
+      <c r="B440" s="44"/>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A441" s="44"/>
+      <c r="B441" s="44"/>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A442" s="44"/>
+      <c r="B442" s="44"/>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A443" s="44"/>
+      <c r="B443" s="44"/>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A444" s="44"/>
+      <c r="B444" s="44"/>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A445" s="44"/>
+      <c r="B445" s="44"/>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A446" s="44"/>
+      <c r="B446" s="44"/>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A447" s="44"/>
+      <c r="B447" s="44"/>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A448" s="44"/>
+      <c r="B448" s="44"/>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A449" s="44"/>
+      <c r="B449" s="44"/>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A450" s="44"/>
+      <c r="B450" s="44"/>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A451" s="44"/>
+      <c r="B451" s="44"/>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A452" s="44"/>
+      <c r="B452" s="44"/>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A453" s="44"/>
+      <c r="B453" s="44"/>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A454" s="44"/>
+      <c r="B454" s="44"/>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A455" s="44"/>
+      <c r="B455" s="44"/>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A456" s="44"/>
+      <c r="B456" s="44"/>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A457" s="44"/>
+      <c r="B457" s="44"/>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A458" s="44"/>
+      <c r="B458" s="44"/>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A459" s="44"/>
+      <c r="B459" s="44"/>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A460" s="44"/>
+      <c r="B460" s="44"/>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A461" s="44"/>
+      <c r="B461" s="44"/>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A462" s="44"/>
+      <c r="B462" s="44"/>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A463" s="44"/>
+      <c r="B463" s="44"/>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A464" s="44"/>
+      <c r="B464" s="44"/>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A465" s="44"/>
+      <c r="B465" s="44"/>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A466" s="44"/>
+      <c r="B466" s="44"/>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A467" s="44"/>
+      <c r="B467" s="44"/>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A468" s="44"/>
+      <c r="B468" s="44"/>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A469" s="44"/>
+      <c r="B469" s="44"/>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A470" s="44"/>
+      <c r="B470" s="44"/>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A471" s="44"/>
+      <c r="B471" s="44"/>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A472" s="44"/>
+      <c r="B472" s="44"/>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A473" s="44"/>
+      <c r="B473" s="44"/>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A474" s="44"/>
+      <c r="B474" s="44"/>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A475" s="44"/>
+      <c r="B475" s="44"/>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A476" s="44"/>
+      <c r="B476" s="44"/>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A477" s="44"/>
+      <c r="B477" s="44"/>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A478" s="44"/>
+      <c r="B478" s="44"/>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A479" s="44"/>
+      <c r="B479" s="44"/>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A480" s="44"/>
+      <c r="B480" s="44"/>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A481" s="44"/>
+      <c r="B481" s="44"/>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A482" s="44"/>
+      <c r="B482" s="44"/>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A483" s="44"/>
+      <c r="B483" s="44"/>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A484" s="44"/>
+      <c r="B484" s="44"/>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A485" s="44"/>
+      <c r="B485" s="44"/>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A486" s="44"/>
+      <c r="B486" s="44"/>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A487" s="44"/>
+      <c r="B487" s="44"/>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A488" s="44"/>
+      <c r="B488" s="44"/>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A489" s="44"/>
+      <c r="B489" s="44"/>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A490" s="44"/>
+      <c r="B490" s="44"/>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A491" s="44"/>
+      <c r="B491" s="44"/>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A492" s="44"/>
+      <c r="B492" s="44"/>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A493" s="44"/>
+      <c r="B493" s="44"/>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A494" s="44"/>
+      <c r="B494" s="44"/>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A495" s="44"/>
+      <c r="B495" s="44"/>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A496" s="44"/>
+      <c r="B496" s="44"/>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A497" s="44"/>
+      <c r="B497" s="44"/>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A498" s="44"/>
+      <c r="B498" s="44"/>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A499" s="44"/>
+      <c r="B499" s="44"/>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A500" s="44"/>
+      <c r="B500" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3B42F4-1841-984B-BE93-9807147BD0DF}">
   <dimension ref="A1:K500"/>
   <sheetViews>
@@ -6644,2150 +8790,6 @@
       <c r="B15" s="44"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
-      <c r="B20" s="44"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="44"/>
-      <c r="B21" s="44"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
-      <c r="B23" s="44"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
-      <c r="B25" s="44"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="44"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
-      <c r="B29" s="44"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
-      <c r="B30" s="44"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="44"/>
-      <c r="B32" s="44"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="44"/>
-      <c r="B34" s="44"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="44"/>
-      <c r="B35" s="44"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="44"/>
-      <c r="B36" s="44"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="44"/>
-      <c r="B37" s="44"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="44"/>
-      <c r="B38" s="44"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="44"/>
-      <c r="B39" s="44"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="44"/>
-      <c r="B40" s="44"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="44"/>
-      <c r="B41" s="44"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="44"/>
-      <c r="B42" s="44"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="44"/>
-      <c r="B43" s="44"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="44"/>
-      <c r="B44" s="44"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="44"/>
-      <c r="B45" s="44"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="44"/>
-      <c r="B46" s="44"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="44"/>
-      <c r="B47" s="44"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="44"/>
-      <c r="B48" s="44"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="44"/>
-      <c r="B49" s="44"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="44"/>
-      <c r="B50" s="44"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="44"/>
-      <c r="B51" s="44"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="44"/>
-      <c r="B52" s="44"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="44"/>
-      <c r="B53" s="44"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="44"/>
-      <c r="B54" s="44"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="44"/>
-      <c r="B55" s="44"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="44"/>
-      <c r="B56" s="44"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="44"/>
-      <c r="B57" s="44"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="44"/>
-      <c r="B58" s="44"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="44"/>
-      <c r="B59" s="44"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="44"/>
-      <c r="B60" s="44"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="44"/>
-      <c r="B61" s="44"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="44"/>
-      <c r="B62" s="44"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="44"/>
-      <c r="B63" s="44"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="44"/>
-      <c r="B64" s="44"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="44"/>
-      <c r="B65" s="44"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="44"/>
-      <c r="B66" s="44"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="44"/>
-      <c r="B67" s="44"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="44"/>
-      <c r="B68" s="44"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="44"/>
-      <c r="B69" s="44"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="44"/>
-      <c r="B70" s="44"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="44"/>
-      <c r="B71" s="44"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="44"/>
-      <c r="B72" s="44"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="44"/>
-      <c r="B73" s="44"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="44"/>
-      <c r="B74" s="44"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="44"/>
-      <c r="B75" s="44"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="44"/>
-      <c r="B76" s="44"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="44"/>
-      <c r="B77" s="44"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="44"/>
-      <c r="B78" s="44"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="44"/>
-      <c r="B79" s="44"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="44"/>
-      <c r="B80" s="44"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="44"/>
-      <c r="B81" s="44"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="44"/>
-      <c r="B82" s="44"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="44"/>
-      <c r="B83" s="44"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="44"/>
-      <c r="B84" s="44"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="44"/>
-      <c r="B85" s="44"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="44"/>
-      <c r="B86" s="44"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="44"/>
-      <c r="B87" s="44"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="44"/>
-      <c r="B88" s="44"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="44"/>
-      <c r="B89" s="44"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="44"/>
-      <c r="B90" s="44"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="44"/>
-      <c r="B91" s="44"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="44"/>
-      <c r="B92" s="44"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="44"/>
-      <c r="B93" s="44"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="44"/>
-      <c r="B94" s="44"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="44"/>
-      <c r="B95" s="44"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="44"/>
-      <c r="B96" s="44"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="44"/>
-      <c r="B97" s="44"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="44"/>
-      <c r="B98" s="44"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="44"/>
-      <c r="B99" s="44"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="44"/>
-      <c r="B100" s="44"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="44"/>
-      <c r="B101" s="44"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="44"/>
-      <c r="B102" s="44"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="44"/>
-      <c r="B103" s="44"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="44"/>
-      <c r="B104" s="44"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="44"/>
-      <c r="B105" s="44"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="44"/>
-      <c r="B106" s="44"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="44"/>
-      <c r="B107" s="44"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="44"/>
-      <c r="B108" s="44"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="44"/>
-      <c r="B109" s="44"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="44"/>
-      <c r="B110" s="44"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="44"/>
-      <c r="B111" s="44"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="44"/>
-      <c r="B112" s="44"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="44"/>
-      <c r="B113" s="44"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="44"/>
-      <c r="B114" s="44"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="44"/>
-      <c r="B115" s="44"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="44"/>
-      <c r="B116" s="44"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="44"/>
-      <c r="B117" s="44"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="44"/>
-      <c r="B118" s="44"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="44"/>
-      <c r="B119" s="44"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="44"/>
-      <c r="B120" s="44"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="44"/>
-      <c r="B121" s="44"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="44"/>
-      <c r="B122" s="44"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="44"/>
-      <c r="B123" s="44"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="44"/>
-      <c r="B124" s="44"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="44"/>
-      <c r="B125" s="44"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="44"/>
-      <c r="B126" s="44"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="44"/>
-      <c r="B127" s="44"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="44"/>
-      <c r="B128" s="44"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="44"/>
-      <c r="B129" s="44"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="44"/>
-      <c r="B130" s="44"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="44"/>
-      <c r="B131" s="44"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="44"/>
-      <c r="B132" s="44"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="44"/>
-      <c r="B133" s="44"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="44"/>
-      <c r="B134" s="44"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="44"/>
-      <c r="B135" s="44"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="44"/>
-      <c r="B136" s="44"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="44"/>
-      <c r="B137" s="44"/>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="44"/>
-      <c r="B138" s="44"/>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="44"/>
-      <c r="B139" s="44"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="44"/>
-      <c r="B140" s="44"/>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="44"/>
-      <c r="B141" s="44"/>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="44"/>
-      <c r="B142" s="44"/>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="44"/>
-      <c r="B143" s="44"/>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="44"/>
-      <c r="B144" s="44"/>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="44"/>
-      <c r="B145" s="44"/>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="44"/>
-      <c r="B146" s="44"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="44"/>
-      <c r="B147" s="44"/>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="44"/>
-      <c r="B148" s="44"/>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="44"/>
-      <c r="B149" s="44"/>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="44"/>
-      <c r="B150" s="44"/>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="44"/>
-      <c r="B151" s="44"/>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="44"/>
-      <c r="B152" s="44"/>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="44"/>
-      <c r="B153" s="44"/>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="44"/>
-      <c r="B154" s="44"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="44"/>
-      <c r="B155" s="44"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="44"/>
-      <c r="B156" s="44"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="44"/>
-      <c r="B157" s="44"/>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="44"/>
-      <c r="B158" s="44"/>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="44"/>
-      <c r="B159" s="44"/>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="44"/>
-      <c r="B160" s="44"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="44"/>
-      <c r="B161" s="44"/>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" s="44"/>
-      <c r="B162" s="44"/>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="44"/>
-      <c r="B163" s="44"/>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" s="44"/>
-      <c r="B164" s="44"/>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" s="44"/>
-      <c r="B165" s="44"/>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="44"/>
-      <c r="B166" s="44"/>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="44"/>
-      <c r="B167" s="44"/>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="44"/>
-      <c r="B168" s="44"/>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" s="44"/>
-      <c r="B169" s="44"/>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" s="44"/>
-      <c r="B170" s="44"/>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" s="44"/>
-      <c r="B171" s="44"/>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="44"/>
-      <c r="B172" s="44"/>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" s="44"/>
-      <c r="B173" s="44"/>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" s="44"/>
-      <c r="B174" s="44"/>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="44"/>
-      <c r="B175" s="44"/>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="44"/>
-      <c r="B176" s="44"/>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="44"/>
-      <c r="B177" s="44"/>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="44"/>
-      <c r="B178" s="44"/>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="44"/>
-      <c r="B179" s="44"/>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="44"/>
-      <c r="B180" s="44"/>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" s="44"/>
-      <c r="B181" s="44"/>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="44"/>
-      <c r="B182" s="44"/>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" s="44"/>
-      <c r="B183" s="44"/>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" s="44"/>
-      <c r="B184" s="44"/>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" s="44"/>
-      <c r="B185" s="44"/>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" s="44"/>
-      <c r="B186" s="44"/>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" s="44"/>
-      <c r="B187" s="44"/>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="44"/>
-      <c r="B188" s="44"/>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" s="44"/>
-      <c r="B189" s="44"/>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="44"/>
-      <c r="B190" s="44"/>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" s="44"/>
-      <c r="B191" s="44"/>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" s="44"/>
-      <c r="B192" s="44"/>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" s="44"/>
-      <c r="B193" s="44"/>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="44"/>
-      <c r="B194" s="44"/>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" s="44"/>
-      <c r="B195" s="44"/>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" s="44"/>
-      <c r="B196" s="44"/>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="44"/>
-      <c r="B197" s="44"/>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" s="44"/>
-      <c r="B198" s="44"/>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="44"/>
-      <c r="B199" s="44"/>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" s="44"/>
-      <c r="B200" s="44"/>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" s="44"/>
-      <c r="B201" s="44"/>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" s="44"/>
-      <c r="B202" s="44"/>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A203" s="44"/>
-      <c r="B203" s="44"/>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="44"/>
-      <c r="B204" s="44"/>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A205" s="44"/>
-      <c r="B205" s="44"/>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A206" s="44"/>
-      <c r="B206" s="44"/>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A207" s="44"/>
-      <c r="B207" s="44"/>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A208" s="44"/>
-      <c r="B208" s="44"/>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" s="44"/>
-      <c r="B209" s="44"/>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" s="44"/>
-      <c r="B210" s="44"/>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A211" s="44"/>
-      <c r="B211" s="44"/>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A212" s="44"/>
-      <c r="B212" s="44"/>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A213" s="44"/>
-      <c r="B213" s="44"/>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A214" s="44"/>
-      <c r="B214" s="44"/>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A215" s="44"/>
-      <c r="B215" s="44"/>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A216" s="44"/>
-      <c r="B216" s="44"/>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A217" s="44"/>
-      <c r="B217" s="44"/>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A218" s="44"/>
-      <c r="B218" s="44"/>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A219" s="44"/>
-      <c r="B219" s="44"/>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A220" s="44"/>
-      <c r="B220" s="44"/>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A221" s="44"/>
-      <c r="B221" s="44"/>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A222" s="44"/>
-      <c r="B222" s="44"/>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A223" s="44"/>
-      <c r="B223" s="44"/>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A224" s="44"/>
-      <c r="B224" s="44"/>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A225" s="44"/>
-      <c r="B225" s="44"/>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A226" s="44"/>
-      <c r="B226" s="44"/>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A227" s="44"/>
-      <c r="B227" s="44"/>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A228" s="44"/>
-      <c r="B228" s="44"/>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" s="44"/>
-      <c r="B229" s="44"/>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" s="44"/>
-      <c r="B230" s="44"/>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A231" s="44"/>
-      <c r="B231" s="44"/>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A232" s="44"/>
-      <c r="B232" s="44"/>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A233" s="44"/>
-      <c r="B233" s="44"/>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A234" s="44"/>
-      <c r="B234" s="44"/>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A235" s="44"/>
-      <c r="B235" s="44"/>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A236" s="44"/>
-      <c r="B236" s="44"/>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A237" s="44"/>
-      <c r="B237" s="44"/>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A238" s="44"/>
-      <c r="B238" s="44"/>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A239" s="44"/>
-      <c r="B239" s="44"/>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A240" s="44"/>
-      <c r="B240" s="44"/>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A241" s="44"/>
-      <c r="B241" s="44"/>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A242" s="44"/>
-      <c r="B242" s="44"/>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A243" s="44"/>
-      <c r="B243" s="44"/>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A244" s="44"/>
-      <c r="B244" s="44"/>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A245" s="44"/>
-      <c r="B245" s="44"/>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A246" s="44"/>
-      <c r="B246" s="44"/>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A247" s="44"/>
-      <c r="B247" s="44"/>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A248" s="44"/>
-      <c r="B248" s="44"/>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A249" s="44"/>
-      <c r="B249" s="44"/>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A250" s="44"/>
-      <c r="B250" s="44"/>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A251" s="44"/>
-      <c r="B251" s="44"/>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A252" s="44"/>
-      <c r="B252" s="44"/>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A253" s="44"/>
-      <c r="B253" s="44"/>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A254" s="44"/>
-      <c r="B254" s="44"/>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A255" s="44"/>
-      <c r="B255" s="44"/>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A256" s="44"/>
-      <c r="B256" s="44"/>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A257" s="44"/>
-      <c r="B257" s="44"/>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A258" s="44"/>
-      <c r="B258" s="44"/>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A259" s="44"/>
-      <c r="B259" s="44"/>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A260" s="44"/>
-      <c r="B260" s="44"/>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A261" s="44"/>
-      <c r="B261" s="44"/>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A262" s="44"/>
-      <c r="B262" s="44"/>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A263" s="44"/>
-      <c r="B263" s="44"/>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A264" s="44"/>
-      <c r="B264" s="44"/>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A265" s="44"/>
-      <c r="B265" s="44"/>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A266" s="44"/>
-      <c r="B266" s="44"/>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A267" s="44"/>
-      <c r="B267" s="44"/>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A268" s="44"/>
-      <c r="B268" s="44"/>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A269" s="44"/>
-      <c r="B269" s="44"/>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A270" s="44"/>
-      <c r="B270" s="44"/>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A271" s="44"/>
-      <c r="B271" s="44"/>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A272" s="44"/>
-      <c r="B272" s="44"/>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A273" s="44"/>
-      <c r="B273" s="44"/>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A274" s="44"/>
-      <c r="B274" s="44"/>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" s="44"/>
-      <c r="B275" s="44"/>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A276" s="44"/>
-      <c r="B276" s="44"/>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" s="44"/>
-      <c r="B277" s="44"/>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A278" s="44"/>
-      <c r="B278" s="44"/>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A279" s="44"/>
-      <c r="B279" s="44"/>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" s="44"/>
-      <c r="B280" s="44"/>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A281" s="44"/>
-      <c r="B281" s="44"/>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A282" s="44"/>
-      <c r="B282" s="44"/>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A283" s="44"/>
-      <c r="B283" s="44"/>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A284" s="44"/>
-      <c r="B284" s="44"/>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A285" s="44"/>
-      <c r="B285" s="44"/>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A286" s="44"/>
-      <c r="B286" s="44"/>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A287" s="44"/>
-      <c r="B287" s="44"/>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A288" s="44"/>
-      <c r="B288" s="44"/>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A289" s="44"/>
-      <c r="B289" s="44"/>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A290" s="44"/>
-      <c r="B290" s="44"/>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A291" s="44"/>
-      <c r="B291" s="44"/>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A292" s="44"/>
-      <c r="B292" s="44"/>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A293" s="44"/>
-      <c r="B293" s="44"/>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A294" s="44"/>
-      <c r="B294" s="44"/>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A295" s="44"/>
-      <c r="B295" s="44"/>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A296" s="44"/>
-      <c r="B296" s="44"/>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A297" s="44"/>
-      <c r="B297" s="44"/>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A298" s="44"/>
-      <c r="B298" s="44"/>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A299" s="44"/>
-      <c r="B299" s="44"/>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A300" s="44"/>
-      <c r="B300" s="44"/>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A301" s="44"/>
-      <c r="B301" s="44"/>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A302" s="44"/>
-      <c r="B302" s="44"/>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A303" s="44"/>
-      <c r="B303" s="44"/>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A304" s="44"/>
-      <c r="B304" s="44"/>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A305" s="44"/>
-      <c r="B305" s="44"/>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A306" s="44"/>
-      <c r="B306" s="44"/>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A307" s="44"/>
-      <c r="B307" s="44"/>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A308" s="44"/>
-      <c r="B308" s="44"/>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A309" s="44"/>
-      <c r="B309" s="44"/>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A310" s="44"/>
-      <c r="B310" s="44"/>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A311" s="44"/>
-      <c r="B311" s="44"/>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A312" s="44"/>
-      <c r="B312" s="44"/>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A313" s="44"/>
-      <c r="B313" s="44"/>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A314" s="44"/>
-      <c r="B314" s="44"/>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A315" s="44"/>
-      <c r="B315" s="44"/>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A316" s="44"/>
-      <c r="B316" s="44"/>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A317" s="44"/>
-      <c r="B317" s="44"/>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A318" s="44"/>
-      <c r="B318" s="44"/>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A319" s="44"/>
-      <c r="B319" s="44"/>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A320" s="44"/>
-      <c r="B320" s="44"/>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A321" s="44"/>
-      <c r="B321" s="44"/>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A322" s="44"/>
-      <c r="B322" s="44"/>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A323" s="44"/>
-      <c r="B323" s="44"/>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A324" s="44"/>
-      <c r="B324" s="44"/>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A325" s="44"/>
-      <c r="B325" s="44"/>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A326" s="44"/>
-      <c r="B326" s="44"/>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A327" s="44"/>
-      <c r="B327" s="44"/>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A328" s="44"/>
-      <c r="B328" s="44"/>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A329" s="44"/>
-      <c r="B329" s="44"/>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A330" s="44"/>
-      <c r="B330" s="44"/>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A331" s="44"/>
-      <c r="B331" s="44"/>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A332" s="44"/>
-      <c r="B332" s="44"/>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A333" s="44"/>
-      <c r="B333" s="44"/>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A334" s="44"/>
-      <c r="B334" s="44"/>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A335" s="44"/>
-      <c r="B335" s="44"/>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A336" s="44"/>
-      <c r="B336" s="44"/>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A337" s="44"/>
-      <c r="B337" s="44"/>
-    </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A338" s="44"/>
-      <c r="B338" s="44"/>
-    </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A339" s="44"/>
-      <c r="B339" s="44"/>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A340" s="44"/>
-      <c r="B340" s="44"/>
-    </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A341" s="44"/>
-      <c r="B341" s="44"/>
-    </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A342" s="44"/>
-      <c r="B342" s="44"/>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A343" s="44"/>
-      <c r="B343" s="44"/>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A344" s="44"/>
-      <c r="B344" s="44"/>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A345" s="44"/>
-      <c r="B345" s="44"/>
-    </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A346" s="44"/>
-      <c r="B346" s="44"/>
-    </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A347" s="44"/>
-      <c r="B347" s="44"/>
-    </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A348" s="44"/>
-      <c r="B348" s="44"/>
-    </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A349" s="44"/>
-      <c r="B349" s="44"/>
-    </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A350" s="44"/>
-      <c r="B350" s="44"/>
-    </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A351" s="44"/>
-      <c r="B351" s="44"/>
-    </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A352" s="44"/>
-      <c r="B352" s="44"/>
-    </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A353" s="44"/>
-      <c r="B353" s="44"/>
-    </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A354" s="44"/>
-      <c r="B354" s="44"/>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A355" s="44"/>
-      <c r="B355" s="44"/>
-    </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A356" s="44"/>
-      <c r="B356" s="44"/>
-    </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A357" s="44"/>
-      <c r="B357" s="44"/>
-    </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A358" s="44"/>
-      <c r="B358" s="44"/>
-    </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A359" s="44"/>
-      <c r="B359" s="44"/>
-    </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A360" s="44"/>
-      <c r="B360" s="44"/>
-    </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A361" s="44"/>
-      <c r="B361" s="44"/>
-    </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A362" s="44"/>
-      <c r="B362" s="44"/>
-    </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A363" s="44"/>
-      <c r="B363" s="44"/>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A364" s="44"/>
-      <c r="B364" s="44"/>
-    </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A365" s="44"/>
-      <c r="B365" s="44"/>
-    </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A366" s="44"/>
-      <c r="B366" s="44"/>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A367" s="44"/>
-      <c r="B367" s="44"/>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A368" s="44"/>
-      <c r="B368" s="44"/>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A369" s="44"/>
-      <c r="B369" s="44"/>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A370" s="44"/>
-      <c r="B370" s="44"/>
-    </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A371" s="44"/>
-      <c r="B371" s="44"/>
-    </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A372" s="44"/>
-      <c r="B372" s="44"/>
-    </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A373" s="44"/>
-      <c r="B373" s="44"/>
-    </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A374" s="44"/>
-      <c r="B374" s="44"/>
-    </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A375" s="44"/>
-      <c r="B375" s="44"/>
-    </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A376" s="44"/>
-      <c r="B376" s="44"/>
-    </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A377" s="44"/>
-      <c r="B377" s="44"/>
-    </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A378" s="44"/>
-      <c r="B378" s="44"/>
-    </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A379" s="44"/>
-      <c r="B379" s="44"/>
-    </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A380" s="44"/>
-      <c r="B380" s="44"/>
-    </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A381" s="44"/>
-      <c r="B381" s="44"/>
-    </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A382" s="44"/>
-      <c r="B382" s="44"/>
-    </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A383" s="44"/>
-      <c r="B383" s="44"/>
-    </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A384" s="44"/>
-      <c r="B384" s="44"/>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A385" s="44"/>
-      <c r="B385" s="44"/>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A386" s="44"/>
-      <c r="B386" s="44"/>
-    </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A387" s="44"/>
-      <c r="B387" s="44"/>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A388" s="44"/>
-      <c r="B388" s="44"/>
-    </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A389" s="44"/>
-      <c r="B389" s="44"/>
-    </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A390" s="44"/>
-      <c r="B390" s="44"/>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A391" s="44"/>
-      <c r="B391" s="44"/>
-    </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A392" s="44"/>
-      <c r="B392" s="44"/>
-    </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A393" s="44"/>
-      <c r="B393" s="44"/>
-    </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A394" s="44"/>
-      <c r="B394" s="44"/>
-    </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A395" s="44"/>
-      <c r="B395" s="44"/>
-    </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A396" s="44"/>
-      <c r="B396" s="44"/>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A397" s="44"/>
-      <c r="B397" s="44"/>
-    </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A398" s="44"/>
-      <c r="B398" s="44"/>
-    </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A399" s="44"/>
-      <c r="B399" s="44"/>
-    </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A400" s="44"/>
-      <c r="B400" s="44"/>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A401" s="44"/>
-      <c r="B401" s="44"/>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A402" s="44"/>
-      <c r="B402" s="44"/>
-    </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A403" s="44"/>
-      <c r="B403" s="44"/>
-    </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A404" s="44"/>
-      <c r="B404" s="44"/>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A405" s="44"/>
-      <c r="B405" s="44"/>
-    </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A406" s="44"/>
-      <c r="B406" s="44"/>
-    </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A407" s="44"/>
-      <c r="B407" s="44"/>
-    </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A408" s="44"/>
-      <c r="B408" s="44"/>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A409" s="44"/>
-      <c r="B409" s="44"/>
-    </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A410" s="44"/>
-      <c r="B410" s="44"/>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A411" s="44"/>
-      <c r="B411" s="44"/>
-    </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A412" s="44"/>
-      <c r="B412" s="44"/>
-    </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A413" s="44"/>
-      <c r="B413" s="44"/>
-    </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A414" s="44"/>
-      <c r="B414" s="44"/>
-    </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A415" s="44"/>
-      <c r="B415" s="44"/>
-    </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A416" s="44"/>
-      <c r="B416" s="44"/>
-    </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A417" s="44"/>
-      <c r="B417" s="44"/>
-    </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A418" s="44"/>
-      <c r="B418" s="44"/>
-    </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A419" s="44"/>
-      <c r="B419" s="44"/>
-    </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A420" s="44"/>
-      <c r="B420" s="44"/>
-    </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A421" s="44"/>
-      <c r="B421" s="44"/>
-    </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A422" s="44"/>
-      <c r="B422" s="44"/>
-    </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A423" s="44"/>
-      <c r="B423" s="44"/>
-    </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A424" s="44"/>
-      <c r="B424" s="44"/>
-    </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A425" s="44"/>
-      <c r="B425" s="44"/>
-    </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A426" s="44"/>
-      <c r="B426" s="44"/>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A427" s="44"/>
-      <c r="B427" s="44"/>
-    </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A428" s="44"/>
-      <c r="B428" s="44"/>
-    </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A429" s="44"/>
-      <c r="B429" s="44"/>
-    </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A430" s="44"/>
-      <c r="B430" s="44"/>
-    </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A431" s="44"/>
-      <c r="B431" s="44"/>
-    </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A432" s="44"/>
-      <c r="B432" s="44"/>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A433" s="44"/>
-      <c r="B433" s="44"/>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A434" s="44"/>
-      <c r="B434" s="44"/>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A435" s="44"/>
-      <c r="B435" s="44"/>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A436" s="44"/>
-      <c r="B436" s="44"/>
-    </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A437" s="44"/>
-      <c r="B437" s="44"/>
-    </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A438" s="44"/>
-      <c r="B438" s="44"/>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A439" s="44"/>
-      <c r="B439" s="44"/>
-    </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A440" s="44"/>
-      <c r="B440" s="44"/>
-    </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A441" s="44"/>
-      <c r="B441" s="44"/>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A442" s="44"/>
-      <c r="B442" s="44"/>
-    </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A443" s="44"/>
-      <c r="B443" s="44"/>
-    </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A444" s="44"/>
-      <c r="B444" s="44"/>
-    </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A445" s="44"/>
-      <c r="B445" s="44"/>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A446" s="44"/>
-      <c r="B446" s="44"/>
-    </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A447" s="44"/>
-      <c r="B447" s="44"/>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A448" s="44"/>
-      <c r="B448" s="44"/>
-    </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A449" s="44"/>
-      <c r="B449" s="44"/>
-    </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A450" s="44"/>
-      <c r="B450" s="44"/>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A451" s="44"/>
-      <c r="B451" s="44"/>
-    </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A452" s="44"/>
-      <c r="B452" s="44"/>
-    </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A453" s="44"/>
-      <c r="B453" s="44"/>
-    </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A454" s="44"/>
-      <c r="B454" s="44"/>
-    </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A455" s="44"/>
-      <c r="B455" s="44"/>
-    </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A456" s="44"/>
-      <c r="B456" s="44"/>
-    </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A457" s="44"/>
-      <c r="B457" s="44"/>
-    </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A458" s="44"/>
-      <c r="B458" s="44"/>
-    </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A459" s="44"/>
-      <c r="B459" s="44"/>
-    </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A460" s="44"/>
-      <c r="B460" s="44"/>
-    </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A461" s="44"/>
-      <c r="B461" s="44"/>
-    </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A462" s="44"/>
-      <c r="B462" s="44"/>
-    </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A463" s="44"/>
-      <c r="B463" s="44"/>
-    </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A464" s="44"/>
-      <c r="B464" s="44"/>
-    </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A465" s="44"/>
-      <c r="B465" s="44"/>
-    </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A466" s="44"/>
-      <c r="B466" s="44"/>
-    </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A467" s="44"/>
-      <c r="B467" s="44"/>
-    </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A468" s="44"/>
-      <c r="B468" s="44"/>
-    </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A469" s="44"/>
-      <c r="B469" s="44"/>
-    </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A470" s="44"/>
-      <c r="B470" s="44"/>
-    </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A471" s="44"/>
-      <c r="B471" s="44"/>
-    </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A472" s="44"/>
-      <c r="B472" s="44"/>
-    </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A473" s="44"/>
-      <c r="B473" s="44"/>
-    </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A474" s="44"/>
-      <c r="B474" s="44"/>
-    </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A475" s="44"/>
-      <c r="B475" s="44"/>
-    </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A476" s="44"/>
-      <c r="B476" s="44"/>
-    </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A477" s="44"/>
-      <c r="B477" s="44"/>
-    </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A478" s="44"/>
-      <c r="B478" s="44"/>
-    </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A479" s="44"/>
-      <c r="B479" s="44"/>
-    </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A480" s="44"/>
-      <c r="B480" s="44"/>
-    </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A481" s="44"/>
-      <c r="B481" s="44"/>
-    </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A482" s="44"/>
-      <c r="B482" s="44"/>
-    </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A483" s="44"/>
-      <c r="B483" s="44"/>
-    </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A484" s="44"/>
-      <c r="B484" s="44"/>
-    </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A485" s="44"/>
-      <c r="B485" s="44"/>
-    </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A486" s="44"/>
-      <c r="B486" s="44"/>
-    </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A487" s="44"/>
-      <c r="B487" s="44"/>
-    </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A488" s="44"/>
-      <c r="B488" s="44"/>
-    </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A489" s="44"/>
-      <c r="B489" s="44"/>
-    </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A490" s="44"/>
-      <c r="B490" s="44"/>
-    </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A491" s="44"/>
-      <c r="B491" s="44"/>
-    </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A492" s="44"/>
-      <c r="B492" s="44"/>
-    </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A493" s="44"/>
-      <c r="B493" s="44"/>
-    </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A494" s="44"/>
-      <c r="B494" s="44"/>
-    </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A495" s="44"/>
-      <c r="B495" s="44"/>
-    </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A496" s="44"/>
-      <c r="B496" s="44"/>
-    </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A497" s="44"/>
-      <c r="B497" s="44"/>
-    </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A498" s="44"/>
-      <c r="B498" s="44"/>
-    </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A499" s="44"/>
-      <c r="B499" s="44"/>
-    </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A500" s="44"/>
-      <c r="B500" s="44"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E2F17F-B09D-944E-9EA4-A1F4C79AA9D1}">
-  <sheetPr codeName="Hoja6"/>
-  <dimension ref="A1:E500"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1205</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D2">
-        <v>8824813</v>
-      </c>
-      <c r="E2">
-        <v>-6875556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>839</v>
-      </c>
-      <c r="C3" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C4" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D5">
-        <v>574118578</v>
-      </c>
-      <c r="E5">
-        <v>3878153423</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D6">
-        <v>4952998587</v>
-      </c>
-      <c r="E6">
-        <v>-4070914402</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>839</v>
-      </c>
-      <c r="C7" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D7">
-        <v>132659301</v>
-      </c>
-      <c r="E7">
-        <v>-134705661</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>1077</v>
-      </c>
-      <c r="C8" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C9" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>852</v>
-      </c>
-      <c r="C10" s="45">
-        <v>45627</v>
-      </c>
-      <c r="D10">
-        <v>13276780</v>
-      </c>
-      <c r="E10">
-        <v>-77831635</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
-      <c r="B11" s="44"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
-      <c r="B12" s="44"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
     </row>
@@ -12324,7 +12326,7 @@
   </sheetPr>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -59408,7 +59410,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -59761,13 +59763,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F504A30D0A8B7C48AC3312637B06038A" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18aa81df5b435925a4ef391b68c25b4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="df0aad82-cca9-4ab3-a26b-b2d93ab652bf" xmlns:ns3="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019c64929386a1d9ec4afd0363aaee9d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -60039,7 +60034,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
@@ -60052,7 +60047,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -60061,15 +60056,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08B7F4E1-123B-49B0-A647-9542B55ED434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -60089,7 +60083,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -60107,10 +60101,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: Corregir errores en query de siniestros de autonomia
</commit_message>
<xml_diff>
--- a/data/segmentacion_autonomia.xlsx
+++ b/data/segmentacion_autonomia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/app-analisis-siniestralidad/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F926EA-2F2C-7C44-9197-CF06657FFAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF2BFA3-F310-0A4B-B9A6-0BE7622A6474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" tabRatio="844" firstSheet="5" activeTab="11" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" tabRatio="844" firstSheet="3" activeTab="11" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Aperturas_Siniestros" sheetId="113" r:id="rId1"/>
@@ -24,8 +24,8 @@
     <sheet name="add_s_Inc_Ced_Atipicos" sheetId="17" r:id="rId9"/>
     <sheet name="Cuadre_Siniestros" sheetId="20" r:id="rId10"/>
     <sheet name="Cuadre_Primas" sheetId="21" r:id="rId11"/>
-    <sheet name="add_s_SAP_Sinis_Ced" sheetId="109" r:id="rId12"/>
-    <sheet name="add_p_SAP_Primas_Ced" sheetId="112" r:id="rId13"/>
+    <sheet name="add_p_SAP_Primas_Ced" sheetId="116" r:id="rId12"/>
+    <sheet name="add_s_SAP_Sinis_Ced" sheetId="109" r:id="rId13"/>
     <sheet name="add_p_Gastos_Expedicion" sheetId="18" r:id="rId14"/>
     <sheet name="Amparos_Negocio_083" sheetId="4" state="hidden" r:id="rId15"/>
   </sheets>
@@ -6235,11 +6235,2365 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45CE485-2624-FB48-93A7-5765859B0896}">
+  <dimension ref="A1:K500"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="44" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="44" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2">
+        <v>202412</v>
+      </c>
+      <c r="D2">
+        <v>184648783</v>
+      </c>
+      <c r="E2">
+        <v>184648783</v>
+      </c>
+      <c r="F2">
+        <v>217797825</v>
+      </c>
+      <c r="G2">
+        <v>217797825</v>
+      </c>
+      <c r="H2">
+        <v>19246958</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>19246958</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="44" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>839</v>
+      </c>
+      <c r="C3">
+        <v>202412</v>
+      </c>
+      <c r="D3">
+        <v>662347303</v>
+      </c>
+      <c r="E3">
+        <v>662347303</v>
+      </c>
+      <c r="F3">
+        <v>701365482</v>
+      </c>
+      <c r="G3">
+        <v>701365482</v>
+      </c>
+      <c r="H3">
+        <v>19983756</v>
+      </c>
+      <c r="I3">
+        <v>-7</v>
+      </c>
+      <c r="J3">
+        <v>19983763</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C4">
+        <v>202412</v>
+      </c>
+      <c r="D4">
+        <v>1427498894</v>
+      </c>
+      <c r="E4">
+        <v>1427498894</v>
+      </c>
+      <c r="F4">
+        <v>1432785215</v>
+      </c>
+      <c r="G4">
+        <v>1432785215</v>
+      </c>
+      <c r="H4">
+        <v>5286321</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>5286321</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5">
+        <v>202412</v>
+      </c>
+      <c r="D5">
+        <v>37620549295</v>
+      </c>
+      <c r="E5">
+        <v>34615671489</v>
+      </c>
+      <c r="F5">
+        <v>39557484565</v>
+      </c>
+      <c r="G5">
+        <v>36552606759</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>3004877806</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6">
+        <v>202412</v>
+      </c>
+      <c r="D6">
+        <v>179132945472</v>
+      </c>
+      <c r="E6">
+        <v>179129728394</v>
+      </c>
+      <c r="F6">
+        <v>157700290763</v>
+      </c>
+      <c r="G6">
+        <v>157697073685</v>
+      </c>
+      <c r="H6">
+        <v>-21234825506</v>
+      </c>
+      <c r="I6">
+        <v>-197829203</v>
+      </c>
+      <c r="J6">
+        <v>-21036996303</v>
+      </c>
+      <c r="K6">
+        <v>3217078</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>839</v>
+      </c>
+      <c r="C7">
+        <v>202412</v>
+      </c>
+      <c r="D7">
+        <v>4564533939</v>
+      </c>
+      <c r="E7">
+        <v>3488760438</v>
+      </c>
+      <c r="F7">
+        <v>4718335471</v>
+      </c>
+      <c r="G7">
+        <v>3642561970</v>
+      </c>
+      <c r="H7">
+        <v>429310584</v>
+      </c>
+      <c r="I7">
+        <v>-275513252</v>
+      </c>
+      <c r="J7">
+        <v>704823836</v>
+      </c>
+      <c r="K7">
+        <v>1075773501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C8">
+        <v>202412</v>
+      </c>
+      <c r="D8">
+        <v>371614941</v>
+      </c>
+      <c r="E8">
+        <v>371614941</v>
+      </c>
+      <c r="F8">
+        <v>512158076</v>
+      </c>
+      <c r="G8">
+        <v>512158076</v>
+      </c>
+      <c r="H8">
+        <v>140543135</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>140543135</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C9">
+        <v>202412</v>
+      </c>
+      <c r="D9">
+        <v>164195594</v>
+      </c>
+      <c r="E9">
+        <v>59067147</v>
+      </c>
+      <c r="F9">
+        <v>166590275</v>
+      </c>
+      <c r="G9">
+        <v>61461828</v>
+      </c>
+      <c r="H9">
+        <v>10612172</v>
+      </c>
+      <c r="I9">
+        <v>-8217491</v>
+      </c>
+      <c r="J9">
+        <v>18829663</v>
+      </c>
+      <c r="K9">
+        <v>105128447</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C10">
+        <v>202412</v>
+      </c>
+      <c r="D10">
+        <v>36755378</v>
+      </c>
+      <c r="E10">
+        <v>36755378</v>
+      </c>
+      <c r="F10">
+        <v>64791487</v>
+      </c>
+      <c r="G10">
+        <v>64791487</v>
+      </c>
+      <c r="H10">
+        <v>28036109</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>28036109</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>852</v>
+      </c>
+      <c r="C11">
+        <v>202412</v>
+      </c>
+      <c r="D11">
+        <v>1924958502</v>
+      </c>
+      <c r="E11">
+        <v>1293352057</v>
+      </c>
+      <c r="F11">
+        <v>1887250085</v>
+      </c>
+      <c r="G11">
+        <v>1255643640</v>
+      </c>
+      <c r="H11">
+        <v>-142440077</v>
+      </c>
+      <c r="I11">
+        <v>104731660</v>
+      </c>
+      <c r="J11">
+        <v>-247171737</v>
+      </c>
+      <c r="K11">
+        <v>631606445</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="44"/>
+      <c r="B28" s="44"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="44"/>
+      <c r="B30" s="44"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="44"/>
+      <c r="B32" s="44"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="44"/>
+      <c r="B33" s="44"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="44"/>
+      <c r="B36" s="44"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="44"/>
+      <c r="B37" s="44"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="44"/>
+      <c r="B38" s="44"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="44"/>
+      <c r="B39" s="44"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="44"/>
+      <c r="B41" s="44"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="44"/>
+      <c r="B45" s="44"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="44"/>
+      <c r="B47" s="44"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="44"/>
+      <c r="B48" s="44"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="44"/>
+      <c r="B49" s="44"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="44"/>
+      <c r="B50" s="44"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="44"/>
+      <c r="B51" s="44"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="44"/>
+      <c r="B52" s="44"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="44"/>
+      <c r="B53" s="44"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="44"/>
+      <c r="B54" s="44"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="44"/>
+      <c r="B55" s="44"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="44"/>
+      <c r="B57" s="44"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="44"/>
+      <c r="B58" s="44"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="44"/>
+      <c r="B59" s="44"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="44"/>
+      <c r="B60" s="44"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="44"/>
+      <c r="B61" s="44"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="44"/>
+      <c r="B62" s="44"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="44"/>
+      <c r="B63" s="44"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="44"/>
+      <c r="B64" s="44"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="44"/>
+      <c r="B65" s="44"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="44"/>
+      <c r="B66" s="44"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="44"/>
+      <c r="B67" s="44"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="44"/>
+      <c r="B68" s="44"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="44"/>
+      <c r="B69" s="44"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="44"/>
+      <c r="B70" s="44"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="44"/>
+      <c r="B71" s="44"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="44"/>
+      <c r="B72" s="44"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="44"/>
+      <c r="B73" s="44"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="44"/>
+      <c r="B74" s="44"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="44"/>
+      <c r="B75" s="44"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="44"/>
+      <c r="B76" s="44"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="44"/>
+      <c r="B77" s="44"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="44"/>
+      <c r="B78" s="44"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="44"/>
+      <c r="B79" s="44"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="44"/>
+      <c r="B80" s="44"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="44"/>
+      <c r="B81" s="44"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="44"/>
+      <c r="B82" s="44"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="44"/>
+      <c r="B86" s="44"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="44"/>
+      <c r="B88" s="44"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="44"/>
+      <c r="B89" s="44"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="44"/>
+      <c r="B90" s="44"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="44"/>
+      <c r="B91" s="44"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="44"/>
+      <c r="B92" s="44"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="44"/>
+      <c r="B93" s="44"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="44"/>
+      <c r="B94" s="44"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="44"/>
+      <c r="B95" s="44"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="44"/>
+      <c r="B96" s="44"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="44"/>
+      <c r="B97" s="44"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="44"/>
+      <c r="B98" s="44"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="44"/>
+      <c r="B99" s="44"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="44"/>
+      <c r="B100" s="44"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="44"/>
+      <c r="B101" s="44"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="44"/>
+      <c r="B102" s="44"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="44"/>
+      <c r="B103" s="44"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="44"/>
+      <c r="B104" s="44"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="44"/>
+      <c r="B105" s="44"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="44"/>
+      <c r="B106" s="44"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="44"/>
+      <c r="B107" s="44"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="44"/>
+      <c r="B108" s="44"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="44"/>
+      <c r="B109" s="44"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="44"/>
+      <c r="B110" s="44"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="44"/>
+      <c r="B111" s="44"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="44"/>
+      <c r="B112" s="44"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="44"/>
+      <c r="B113" s="44"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="44"/>
+      <c r="B114" s="44"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="44"/>
+      <c r="B115" s="44"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="44"/>
+      <c r="B116" s="44"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="44"/>
+      <c r="B117" s="44"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="44"/>
+      <c r="B118" s="44"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="44"/>
+      <c r="B119" s="44"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="44"/>
+      <c r="B120" s="44"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="44"/>
+      <c r="B121" s="44"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="44"/>
+      <c r="B122" s="44"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="44"/>
+      <c r="B123" s="44"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="44"/>
+      <c r="B124" s="44"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="44"/>
+      <c r="B125" s="44"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="44"/>
+      <c r="B126" s="44"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="44"/>
+      <c r="B127" s="44"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="44"/>
+      <c r="B128" s="44"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="44"/>
+      <c r="B129" s="44"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="44"/>
+      <c r="B130" s="44"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="44"/>
+      <c r="B131" s="44"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="44"/>
+      <c r="B132" s="44"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="44"/>
+      <c r="B133" s="44"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="44"/>
+      <c r="B134" s="44"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="44"/>
+      <c r="B135" s="44"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="44"/>
+      <c r="B136" s="44"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="44"/>
+      <c r="B137" s="44"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="44"/>
+      <c r="B138" s="44"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="44"/>
+      <c r="B139" s="44"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="44"/>
+      <c r="B140" s="44"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="44"/>
+      <c r="B141" s="44"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="44"/>
+      <c r="B142" s="44"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="44"/>
+      <c r="B143" s="44"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="44"/>
+      <c r="B144" s="44"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="44"/>
+      <c r="B145" s="44"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="44"/>
+      <c r="B146" s="44"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="44"/>
+      <c r="B147" s="44"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="44"/>
+      <c r="B148" s="44"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="44"/>
+      <c r="B149" s="44"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="44"/>
+      <c r="B150" s="44"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="44"/>
+      <c r="B151" s="44"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="44"/>
+      <c r="B152" s="44"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="44"/>
+      <c r="B153" s="44"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="44"/>
+      <c r="B154" s="44"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="44"/>
+      <c r="B155" s="44"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="44"/>
+      <c r="B156" s="44"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="44"/>
+      <c r="B157" s="44"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="44"/>
+      <c r="B158" s="44"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="44"/>
+      <c r="B159" s="44"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="44"/>
+      <c r="B160" s="44"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="44"/>
+      <c r="B161" s="44"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="44"/>
+      <c r="B162" s="44"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="44"/>
+      <c r="B163" s="44"/>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="44"/>
+      <c r="B164" s="44"/>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="44"/>
+      <c r="B165" s="44"/>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="44"/>
+      <c r="B166" s="44"/>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="44"/>
+      <c r="B167" s="44"/>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="44"/>
+      <c r="B168" s="44"/>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="44"/>
+      <c r="B169" s="44"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="44"/>
+      <c r="B170" s="44"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="44"/>
+      <c r="B171" s="44"/>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="44"/>
+      <c r="B172" s="44"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="44"/>
+      <c r="B173" s="44"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="44"/>
+      <c r="B174" s="44"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="44"/>
+      <c r="B175" s="44"/>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="44"/>
+      <c r="B176" s="44"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="44"/>
+      <c r="B177" s="44"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="44"/>
+      <c r="B178" s="44"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="44"/>
+      <c r="B179" s="44"/>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="44"/>
+      <c r="B180" s="44"/>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="44"/>
+      <c r="B181" s="44"/>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="44"/>
+      <c r="B182" s="44"/>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="44"/>
+      <c r="B183" s="44"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="44"/>
+      <c r="B184" s="44"/>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="44"/>
+      <c r="B185" s="44"/>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="44"/>
+      <c r="B186" s="44"/>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="44"/>
+      <c r="B187" s="44"/>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="44"/>
+      <c r="B188" s="44"/>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="44"/>
+      <c r="B189" s="44"/>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="44"/>
+      <c r="B190" s="44"/>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="44"/>
+      <c r="B191" s="44"/>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="44"/>
+      <c r="B192" s="44"/>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="44"/>
+      <c r="B193" s="44"/>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="44"/>
+      <c r="B194" s="44"/>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="44"/>
+      <c r="B195" s="44"/>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="44"/>
+      <c r="B196" s="44"/>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="44"/>
+      <c r="B197" s="44"/>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="44"/>
+      <c r="B198" s="44"/>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="44"/>
+      <c r="B199" s="44"/>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="44"/>
+      <c r="B200" s="44"/>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="44"/>
+      <c r="B201" s="44"/>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="44"/>
+      <c r="B202" s="44"/>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="44"/>
+      <c r="B203" s="44"/>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="44"/>
+      <c r="B204" s="44"/>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="44"/>
+      <c r="B205" s="44"/>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="44"/>
+      <c r="B206" s="44"/>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="44"/>
+      <c r="B207" s="44"/>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="44"/>
+      <c r="B208" s="44"/>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="44"/>
+      <c r="B209" s="44"/>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="44"/>
+      <c r="B210" s="44"/>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="44"/>
+      <c r="B211" s="44"/>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="44"/>
+      <c r="B212" s="44"/>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="44"/>
+      <c r="B213" s="44"/>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="44"/>
+      <c r="B214" s="44"/>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="44"/>
+      <c r="B215" s="44"/>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="44"/>
+      <c r="B216" s="44"/>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="44"/>
+      <c r="B217" s="44"/>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="44"/>
+      <c r="B218" s="44"/>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="44"/>
+      <c r="B219" s="44"/>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="44"/>
+      <c r="B220" s="44"/>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="44"/>
+      <c r="B221" s="44"/>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="44"/>
+      <c r="B222" s="44"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="44"/>
+      <c r="B223" s="44"/>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="44"/>
+      <c r="B224" s="44"/>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="44"/>
+      <c r="B225" s="44"/>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="44"/>
+      <c r="B226" s="44"/>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="44"/>
+      <c r="B227" s="44"/>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="44"/>
+      <c r="B228" s="44"/>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="44"/>
+      <c r="B229" s="44"/>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="44"/>
+      <c r="B230" s="44"/>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="44"/>
+      <c r="B231" s="44"/>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="44"/>
+      <c r="B232" s="44"/>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="44"/>
+      <c r="B233" s="44"/>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="44"/>
+      <c r="B234" s="44"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" s="44"/>
+      <c r="B235" s="44"/>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="44"/>
+      <c r="B236" s="44"/>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="44"/>
+      <c r="B237" s="44"/>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="44"/>
+      <c r="B238" s="44"/>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="44"/>
+      <c r="B239" s="44"/>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="44"/>
+      <c r="B240" s="44"/>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="44"/>
+      <c r="B241" s="44"/>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="44"/>
+      <c r="B242" s="44"/>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" s="44"/>
+      <c r="B243" s="44"/>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="44"/>
+      <c r="B244" s="44"/>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="44"/>
+      <c r="B245" s="44"/>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" s="44"/>
+      <c r="B246" s="44"/>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="44"/>
+      <c r="B247" s="44"/>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="44"/>
+      <c r="B248" s="44"/>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="44"/>
+      <c r="B249" s="44"/>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="44"/>
+      <c r="B250" s="44"/>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" s="44"/>
+      <c r="B251" s="44"/>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" s="44"/>
+      <c r="B252" s="44"/>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" s="44"/>
+      <c r="B253" s="44"/>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" s="44"/>
+      <c r="B254" s="44"/>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" s="44"/>
+      <c r="B255" s="44"/>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" s="44"/>
+      <c r="B256" s="44"/>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257" s="44"/>
+      <c r="B257" s="44"/>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258" s="44"/>
+      <c r="B258" s="44"/>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259" s="44"/>
+      <c r="B259" s="44"/>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260" s="44"/>
+      <c r="B260" s="44"/>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" s="44"/>
+      <c r="B261" s="44"/>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" s="44"/>
+      <c r="B262" s="44"/>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263" s="44"/>
+      <c r="B263" s="44"/>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264" s="44"/>
+      <c r="B264" s="44"/>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" s="44"/>
+      <c r="B265" s="44"/>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" s="44"/>
+      <c r="B266" s="44"/>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267" s="44"/>
+      <c r="B267" s="44"/>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268" s="44"/>
+      <c r="B268" s="44"/>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269" s="44"/>
+      <c r="B269" s="44"/>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270" s="44"/>
+      <c r="B270" s="44"/>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" s="44"/>
+      <c r="B271" s="44"/>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272" s="44"/>
+      <c r="B272" s="44"/>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273" s="44"/>
+      <c r="B273" s="44"/>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" s="44"/>
+      <c r="B274" s="44"/>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275" s="44"/>
+      <c r="B275" s="44"/>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" s="44"/>
+      <c r="B276" s="44"/>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" s="44"/>
+      <c r="B277" s="44"/>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" s="44"/>
+      <c r="B278" s="44"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="44"/>
+      <c r="B279" s="44"/>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="44"/>
+      <c r="B280" s="44"/>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="44"/>
+      <c r="B281" s="44"/>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="44"/>
+      <c r="B282" s="44"/>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" s="44"/>
+      <c r="B283" s="44"/>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="44"/>
+      <c r="B284" s="44"/>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" s="44"/>
+      <c r="B285" s="44"/>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286" s="44"/>
+      <c r="B286" s="44"/>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" s="44"/>
+      <c r="B287" s="44"/>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288" s="44"/>
+      <c r="B288" s="44"/>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A289" s="44"/>
+      <c r="B289" s="44"/>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" s="44"/>
+      <c r="B290" s="44"/>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A291" s="44"/>
+      <c r="B291" s="44"/>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A292" s="44"/>
+      <c r="B292" s="44"/>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A293" s="44"/>
+      <c r="B293" s="44"/>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A294" s="44"/>
+      <c r="B294" s="44"/>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A295" s="44"/>
+      <c r="B295" s="44"/>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A296" s="44"/>
+      <c r="B296" s="44"/>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A297" s="44"/>
+      <c r="B297" s="44"/>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A298" s="44"/>
+      <c r="B298" s="44"/>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A299" s="44"/>
+      <c r="B299" s="44"/>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A300" s="44"/>
+      <c r="B300" s="44"/>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A301" s="44"/>
+      <c r="B301" s="44"/>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A302" s="44"/>
+      <c r="B302" s="44"/>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A303" s="44"/>
+      <c r="B303" s="44"/>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A304" s="44"/>
+      <c r="B304" s="44"/>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A305" s="44"/>
+      <c r="B305" s="44"/>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A306" s="44"/>
+      <c r="B306" s="44"/>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A307" s="44"/>
+      <c r="B307" s="44"/>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A308" s="44"/>
+      <c r="B308" s="44"/>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A309" s="44"/>
+      <c r="B309" s="44"/>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A310" s="44"/>
+      <c r="B310" s="44"/>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A311" s="44"/>
+      <c r="B311" s="44"/>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A312" s="44"/>
+      <c r="B312" s="44"/>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A313" s="44"/>
+      <c r="B313" s="44"/>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A314" s="44"/>
+      <c r="B314" s="44"/>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A315" s="44"/>
+      <c r="B315" s="44"/>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A316" s="44"/>
+      <c r="B316" s="44"/>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A317" s="44"/>
+      <c r="B317" s="44"/>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A318" s="44"/>
+      <c r="B318" s="44"/>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A319" s="44"/>
+      <c r="B319" s="44"/>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A320" s="44"/>
+      <c r="B320" s="44"/>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" s="44"/>
+      <c r="B321" s="44"/>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" s="44"/>
+      <c r="B322" s="44"/>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A323" s="44"/>
+      <c r="B323" s="44"/>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A324" s="44"/>
+      <c r="B324" s="44"/>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A325" s="44"/>
+      <c r="B325" s="44"/>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A326" s="44"/>
+      <c r="B326" s="44"/>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A327" s="44"/>
+      <c r="B327" s="44"/>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A328" s="44"/>
+      <c r="B328" s="44"/>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A329" s="44"/>
+      <c r="B329" s="44"/>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A330" s="44"/>
+      <c r="B330" s="44"/>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A331" s="44"/>
+      <c r="B331" s="44"/>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A332" s="44"/>
+      <c r="B332" s="44"/>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A333" s="44"/>
+      <c r="B333" s="44"/>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A334" s="44"/>
+      <c r="B334" s="44"/>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A335" s="44"/>
+      <c r="B335" s="44"/>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A336" s="44"/>
+      <c r="B336" s="44"/>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A337" s="44"/>
+      <c r="B337" s="44"/>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A338" s="44"/>
+      <c r="B338" s="44"/>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A339" s="44"/>
+      <c r="B339" s="44"/>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A340" s="44"/>
+      <c r="B340" s="44"/>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A341" s="44"/>
+      <c r="B341" s="44"/>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A342" s="44"/>
+      <c r="B342" s="44"/>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A343" s="44"/>
+      <c r="B343" s="44"/>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A344" s="44"/>
+      <c r="B344" s="44"/>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A345" s="44"/>
+      <c r="B345" s="44"/>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A346" s="44"/>
+      <c r="B346" s="44"/>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A347" s="44"/>
+      <c r="B347" s="44"/>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A348" s="44"/>
+      <c r="B348" s="44"/>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A349" s="44"/>
+      <c r="B349" s="44"/>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A350" s="44"/>
+      <c r="B350" s="44"/>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A351" s="44"/>
+      <c r="B351" s="44"/>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A352" s="44"/>
+      <c r="B352" s="44"/>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A353" s="44"/>
+      <c r="B353" s="44"/>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A354" s="44"/>
+      <c r="B354" s="44"/>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A355" s="44"/>
+      <c r="B355" s="44"/>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A356" s="44"/>
+      <c r="B356" s="44"/>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A357" s="44"/>
+      <c r="B357" s="44"/>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A358" s="44"/>
+      <c r="B358" s="44"/>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A359" s="44"/>
+      <c r="B359" s="44"/>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A360" s="44"/>
+      <c r="B360" s="44"/>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A361" s="44"/>
+      <c r="B361" s="44"/>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A362" s="44"/>
+      <c r="B362" s="44"/>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A363" s="44"/>
+      <c r="B363" s="44"/>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A364" s="44"/>
+      <c r="B364" s="44"/>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A365" s="44"/>
+      <c r="B365" s="44"/>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A366" s="44"/>
+      <c r="B366" s="44"/>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A367" s="44"/>
+      <c r="B367" s="44"/>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A368" s="44"/>
+      <c r="B368" s="44"/>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A369" s="44"/>
+      <c r="B369" s="44"/>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A370" s="44"/>
+      <c r="B370" s="44"/>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A371" s="44"/>
+      <c r="B371" s="44"/>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A372" s="44"/>
+      <c r="B372" s="44"/>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A373" s="44"/>
+      <c r="B373" s="44"/>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A374" s="44"/>
+      <c r="B374" s="44"/>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A375" s="44"/>
+      <c r="B375" s="44"/>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A376" s="44"/>
+      <c r="B376" s="44"/>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A377" s="44"/>
+      <c r="B377" s="44"/>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A378" s="44"/>
+      <c r="B378" s="44"/>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A379" s="44"/>
+      <c r="B379" s="44"/>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A380" s="44"/>
+      <c r="B380" s="44"/>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A381" s="44"/>
+      <c r="B381" s="44"/>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A382" s="44"/>
+      <c r="B382" s="44"/>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A383" s="44"/>
+      <c r="B383" s="44"/>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A384" s="44"/>
+      <c r="B384" s="44"/>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A385" s="44"/>
+      <c r="B385" s="44"/>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A386" s="44"/>
+      <c r="B386" s="44"/>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A387" s="44"/>
+      <c r="B387" s="44"/>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A388" s="44"/>
+      <c r="B388" s="44"/>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A389" s="44"/>
+      <c r="B389" s="44"/>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A390" s="44"/>
+      <c r="B390" s="44"/>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A391" s="44"/>
+      <c r="B391" s="44"/>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A392" s="44"/>
+      <c r="B392" s="44"/>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A393" s="44"/>
+      <c r="B393" s="44"/>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A394" s="44"/>
+      <c r="B394" s="44"/>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A395" s="44"/>
+      <c r="B395" s="44"/>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A396" s="44"/>
+      <c r="B396" s="44"/>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A397" s="44"/>
+      <c r="B397" s="44"/>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A398" s="44"/>
+      <c r="B398" s="44"/>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A399" s="44"/>
+      <c r="B399" s="44"/>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A400" s="44"/>
+      <c r="B400" s="44"/>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A401" s="44"/>
+      <c r="B401" s="44"/>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A402" s="44"/>
+      <c r="B402" s="44"/>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A403" s="44"/>
+      <c r="B403" s="44"/>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A404" s="44"/>
+      <c r="B404" s="44"/>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A405" s="44"/>
+      <c r="B405" s="44"/>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A406" s="44"/>
+      <c r="B406" s="44"/>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A407" s="44"/>
+      <c r="B407" s="44"/>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A408" s="44"/>
+      <c r="B408" s="44"/>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A409" s="44"/>
+      <c r="B409" s="44"/>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A410" s="44"/>
+      <c r="B410" s="44"/>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A411" s="44"/>
+      <c r="B411" s="44"/>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A412" s="44"/>
+      <c r="B412" s="44"/>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A413" s="44"/>
+      <c r="B413" s="44"/>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A414" s="44"/>
+      <c r="B414" s="44"/>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A415" s="44"/>
+      <c r="B415" s="44"/>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A416" s="44"/>
+      <c r="B416" s="44"/>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A417" s="44"/>
+      <c r="B417" s="44"/>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A418" s="44"/>
+      <c r="B418" s="44"/>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A419" s="44"/>
+      <c r="B419" s="44"/>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A420" s="44"/>
+      <c r="B420" s="44"/>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A421" s="44"/>
+      <c r="B421" s="44"/>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A422" s="44"/>
+      <c r="B422" s="44"/>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A423" s="44"/>
+      <c r="B423" s="44"/>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A424" s="44"/>
+      <c r="B424" s="44"/>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A425" s="44"/>
+      <c r="B425" s="44"/>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A426" s="44"/>
+      <c r="B426" s="44"/>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A427" s="44"/>
+      <c r="B427" s="44"/>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A428" s="44"/>
+      <c r="B428" s="44"/>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A429" s="44"/>
+      <c r="B429" s="44"/>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A430" s="44"/>
+      <c r="B430" s="44"/>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A431" s="44"/>
+      <c r="B431" s="44"/>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A432" s="44"/>
+      <c r="B432" s="44"/>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A433" s="44"/>
+      <c r="B433" s="44"/>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A434" s="44"/>
+      <c r="B434" s="44"/>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A435" s="44"/>
+      <c r="B435" s="44"/>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A436" s="44"/>
+      <c r="B436" s="44"/>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A437" s="44"/>
+      <c r="B437" s="44"/>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A438" s="44"/>
+      <c r="B438" s="44"/>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A439" s="44"/>
+      <c r="B439" s="44"/>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A440" s="44"/>
+      <c r="B440" s="44"/>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A441" s="44"/>
+      <c r="B441" s="44"/>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A442" s="44"/>
+      <c r="B442" s="44"/>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A443" s="44"/>
+      <c r="B443" s="44"/>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A444" s="44"/>
+      <c r="B444" s="44"/>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A445" s="44"/>
+      <c r="B445" s="44"/>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A446" s="44"/>
+      <c r="B446" s="44"/>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A447" s="44"/>
+      <c r="B447" s="44"/>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A448" s="44"/>
+      <c r="B448" s="44"/>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A449" s="44"/>
+      <c r="B449" s="44"/>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A450" s="44"/>
+      <c r="B450" s="44"/>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A451" s="44"/>
+      <c r="B451" s="44"/>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A452" s="44"/>
+      <c r="B452" s="44"/>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A453" s="44"/>
+      <c r="B453" s="44"/>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A454" s="44"/>
+      <c r="B454" s="44"/>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A455" s="44"/>
+      <c r="B455" s="44"/>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A456" s="44"/>
+      <c r="B456" s="44"/>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A457" s="44"/>
+      <c r="B457" s="44"/>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A458" s="44"/>
+      <c r="B458" s="44"/>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A459" s="44"/>
+      <c r="B459" s="44"/>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A460" s="44"/>
+      <c r="B460" s="44"/>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A461" s="44"/>
+      <c r="B461" s="44"/>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A462" s="44"/>
+      <c r="B462" s="44"/>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A463" s="44"/>
+      <c r="B463" s="44"/>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A464" s="44"/>
+      <c r="B464" s="44"/>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A465" s="44"/>
+      <c r="B465" s="44"/>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A466" s="44"/>
+      <c r="B466" s="44"/>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A467" s="44"/>
+      <c r="B467" s="44"/>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A468" s="44"/>
+      <c r="B468" s="44"/>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A469" s="44"/>
+      <c r="B469" s="44"/>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A470" s="44"/>
+      <c r="B470" s="44"/>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A471" s="44"/>
+      <c r="B471" s="44"/>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A472" s="44"/>
+      <c r="B472" s="44"/>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A473" s="44"/>
+      <c r="B473" s="44"/>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A474" s="44"/>
+      <c r="B474" s="44"/>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A475" s="44"/>
+      <c r="B475" s="44"/>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A476" s="44"/>
+      <c r="B476" s="44"/>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A477" s="44"/>
+      <c r="B477" s="44"/>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A478" s="44"/>
+      <c r="B478" s="44"/>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A479" s="44"/>
+      <c r="B479" s="44"/>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A480" s="44"/>
+      <c r="B480" s="44"/>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A481" s="44"/>
+      <c r="B481" s="44"/>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A482" s="44"/>
+      <c r="B482" s="44"/>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A483" s="44"/>
+      <c r="B483" s="44"/>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A484" s="44"/>
+      <c r="B484" s="44"/>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A485" s="44"/>
+      <c r="B485" s="44"/>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A486" s="44"/>
+      <c r="B486" s="44"/>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A487" s="44"/>
+      <c r="B487" s="44"/>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A488" s="44"/>
+      <c r="B488" s="44"/>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A489" s="44"/>
+      <c r="B489" s="44"/>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A490" s="44"/>
+      <c r="B490" s="44"/>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A491" s="44"/>
+      <c r="B491" s="44"/>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A492" s="44"/>
+      <c r="B492" s="44"/>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A493" s="44"/>
+      <c r="B493" s="44"/>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A494" s="44"/>
+      <c r="B494" s="44"/>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A495" s="44"/>
+      <c r="B495" s="44"/>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A496" s="44"/>
+      <c r="B496" s="44"/>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A497" s="44"/>
+      <c r="B497" s="44"/>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A498" s="44"/>
+      <c r="B498" s="44"/>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A499" s="44"/>
+      <c r="B499" s="44"/>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A500" s="44"/>
+      <c r="B500" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E2F17F-B09D-944E-9EA4-A1F4C79AA9D1}">
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -6436,2360 +8790,6 @@
       <c r="B15" s="44"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
-      <c r="B20" s="44"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="44"/>
-      <c r="B21" s="44"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
-      <c r="B23" s="44"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
-      <c r="B25" s="44"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="44"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
-      <c r="B29" s="44"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
-      <c r="B30" s="44"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="44"/>
-      <c r="B32" s="44"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="44"/>
-      <c r="B34" s="44"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="44"/>
-      <c r="B35" s="44"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="44"/>
-      <c r="B36" s="44"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="44"/>
-      <c r="B37" s="44"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="44"/>
-      <c r="B38" s="44"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="44"/>
-      <c r="B39" s="44"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="44"/>
-      <c r="B40" s="44"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="44"/>
-      <c r="B41" s="44"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="44"/>
-      <c r="B42" s="44"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="44"/>
-      <c r="B43" s="44"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="44"/>
-      <c r="B44" s="44"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="44"/>
-      <c r="B45" s="44"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="44"/>
-      <c r="B46" s="44"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="44"/>
-      <c r="B47" s="44"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="44"/>
-      <c r="B48" s="44"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="44"/>
-      <c r="B49" s="44"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="44"/>
-      <c r="B50" s="44"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="44"/>
-      <c r="B51" s="44"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="44"/>
-      <c r="B52" s="44"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="44"/>
-      <c r="B53" s="44"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="44"/>
-      <c r="B54" s="44"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="44"/>
-      <c r="B55" s="44"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="44"/>
-      <c r="B56" s="44"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="44"/>
-      <c r="B57" s="44"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="44"/>
-      <c r="B58" s="44"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="44"/>
-      <c r="B59" s="44"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="44"/>
-      <c r="B60" s="44"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="44"/>
-      <c r="B61" s="44"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="44"/>
-      <c r="B62" s="44"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="44"/>
-      <c r="B63" s="44"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="44"/>
-      <c r="B64" s="44"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="44"/>
-      <c r="B65" s="44"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="44"/>
-      <c r="B66" s="44"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="44"/>
-      <c r="B67" s="44"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="44"/>
-      <c r="B68" s="44"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="44"/>
-      <c r="B69" s="44"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="44"/>
-      <c r="B70" s="44"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="44"/>
-      <c r="B71" s="44"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="44"/>
-      <c r="B72" s="44"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="44"/>
-      <c r="B73" s="44"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="44"/>
-      <c r="B74" s="44"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="44"/>
-      <c r="B75" s="44"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="44"/>
-      <c r="B76" s="44"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="44"/>
-      <c r="B77" s="44"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="44"/>
-      <c r="B78" s="44"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="44"/>
-      <c r="B79" s="44"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="44"/>
-      <c r="B80" s="44"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="44"/>
-      <c r="B81" s="44"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="44"/>
-      <c r="B82" s="44"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="44"/>
-      <c r="B83" s="44"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="44"/>
-      <c r="B84" s="44"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="44"/>
-      <c r="B85" s="44"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="44"/>
-      <c r="B86" s="44"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="44"/>
-      <c r="B87" s="44"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="44"/>
-      <c r="B88" s="44"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="44"/>
-      <c r="B89" s="44"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="44"/>
-      <c r="B90" s="44"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="44"/>
-      <c r="B91" s="44"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="44"/>
-      <c r="B92" s="44"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="44"/>
-      <c r="B93" s="44"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="44"/>
-      <c r="B94" s="44"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="44"/>
-      <c r="B95" s="44"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="44"/>
-      <c r="B96" s="44"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="44"/>
-      <c r="B97" s="44"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="44"/>
-      <c r="B98" s="44"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="44"/>
-      <c r="B99" s="44"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="44"/>
-      <c r="B100" s="44"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="44"/>
-      <c r="B101" s="44"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="44"/>
-      <c r="B102" s="44"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="44"/>
-      <c r="B103" s="44"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="44"/>
-      <c r="B104" s="44"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="44"/>
-      <c r="B105" s="44"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="44"/>
-      <c r="B106" s="44"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="44"/>
-      <c r="B107" s="44"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="44"/>
-      <c r="B108" s="44"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="44"/>
-      <c r="B109" s="44"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="44"/>
-      <c r="B110" s="44"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="44"/>
-      <c r="B111" s="44"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="44"/>
-      <c r="B112" s="44"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="44"/>
-      <c r="B113" s="44"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="44"/>
-      <c r="B114" s="44"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="44"/>
-      <c r="B115" s="44"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="44"/>
-      <c r="B116" s="44"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="44"/>
-      <c r="B117" s="44"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="44"/>
-      <c r="B118" s="44"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="44"/>
-      <c r="B119" s="44"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="44"/>
-      <c r="B120" s="44"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="44"/>
-      <c r="B121" s="44"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="44"/>
-      <c r="B122" s="44"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="44"/>
-      <c r="B123" s="44"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="44"/>
-      <c r="B124" s="44"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="44"/>
-      <c r="B125" s="44"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="44"/>
-      <c r="B126" s="44"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="44"/>
-      <c r="B127" s="44"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="44"/>
-      <c r="B128" s="44"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="44"/>
-      <c r="B129" s="44"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="44"/>
-      <c r="B130" s="44"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="44"/>
-      <c r="B131" s="44"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="44"/>
-      <c r="B132" s="44"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="44"/>
-      <c r="B133" s="44"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="44"/>
-      <c r="B134" s="44"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="44"/>
-      <c r="B135" s="44"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="44"/>
-      <c r="B136" s="44"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="44"/>
-      <c r="B137" s="44"/>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="44"/>
-      <c r="B138" s="44"/>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="44"/>
-      <c r="B139" s="44"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="44"/>
-      <c r="B140" s="44"/>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="44"/>
-      <c r="B141" s="44"/>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="44"/>
-      <c r="B142" s="44"/>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="44"/>
-      <c r="B143" s="44"/>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="44"/>
-      <c r="B144" s="44"/>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="44"/>
-      <c r="B145" s="44"/>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="44"/>
-      <c r="B146" s="44"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="44"/>
-      <c r="B147" s="44"/>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="44"/>
-      <c r="B148" s="44"/>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="44"/>
-      <c r="B149" s="44"/>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="44"/>
-      <c r="B150" s="44"/>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="44"/>
-      <c r="B151" s="44"/>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="44"/>
-      <c r="B152" s="44"/>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="44"/>
-      <c r="B153" s="44"/>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="44"/>
-      <c r="B154" s="44"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="44"/>
-      <c r="B155" s="44"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="44"/>
-      <c r="B156" s="44"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="44"/>
-      <c r="B157" s="44"/>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="44"/>
-      <c r="B158" s="44"/>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="44"/>
-      <c r="B159" s="44"/>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="44"/>
-      <c r="B160" s="44"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="44"/>
-      <c r="B161" s="44"/>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" s="44"/>
-      <c r="B162" s="44"/>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="44"/>
-      <c r="B163" s="44"/>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" s="44"/>
-      <c r="B164" s="44"/>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" s="44"/>
-      <c r="B165" s="44"/>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="44"/>
-      <c r="B166" s="44"/>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="44"/>
-      <c r="B167" s="44"/>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="44"/>
-      <c r="B168" s="44"/>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" s="44"/>
-      <c r="B169" s="44"/>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" s="44"/>
-      <c r="B170" s="44"/>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" s="44"/>
-      <c r="B171" s="44"/>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="44"/>
-      <c r="B172" s="44"/>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" s="44"/>
-      <c r="B173" s="44"/>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" s="44"/>
-      <c r="B174" s="44"/>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="44"/>
-      <c r="B175" s="44"/>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="44"/>
-      <c r="B176" s="44"/>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="44"/>
-      <c r="B177" s="44"/>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="44"/>
-      <c r="B178" s="44"/>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="44"/>
-      <c r="B179" s="44"/>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="44"/>
-      <c r="B180" s="44"/>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" s="44"/>
-      <c r="B181" s="44"/>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="44"/>
-      <c r="B182" s="44"/>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" s="44"/>
-      <c r="B183" s="44"/>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" s="44"/>
-      <c r="B184" s="44"/>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" s="44"/>
-      <c r="B185" s="44"/>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" s="44"/>
-      <c r="B186" s="44"/>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" s="44"/>
-      <c r="B187" s="44"/>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="44"/>
-      <c r="B188" s="44"/>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" s="44"/>
-      <c r="B189" s="44"/>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="44"/>
-      <c r="B190" s="44"/>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" s="44"/>
-      <c r="B191" s="44"/>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" s="44"/>
-      <c r="B192" s="44"/>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" s="44"/>
-      <c r="B193" s="44"/>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="44"/>
-      <c r="B194" s="44"/>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" s="44"/>
-      <c r="B195" s="44"/>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" s="44"/>
-      <c r="B196" s="44"/>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="44"/>
-      <c r="B197" s="44"/>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" s="44"/>
-      <c r="B198" s="44"/>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="44"/>
-      <c r="B199" s="44"/>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" s="44"/>
-      <c r="B200" s="44"/>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" s="44"/>
-      <c r="B201" s="44"/>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" s="44"/>
-      <c r="B202" s="44"/>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A203" s="44"/>
-      <c r="B203" s="44"/>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="44"/>
-      <c r="B204" s="44"/>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A205" s="44"/>
-      <c r="B205" s="44"/>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A206" s="44"/>
-      <c r="B206" s="44"/>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A207" s="44"/>
-      <c r="B207" s="44"/>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A208" s="44"/>
-      <c r="B208" s="44"/>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" s="44"/>
-      <c r="B209" s="44"/>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" s="44"/>
-      <c r="B210" s="44"/>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A211" s="44"/>
-      <c r="B211" s="44"/>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A212" s="44"/>
-      <c r="B212" s="44"/>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A213" s="44"/>
-      <c r="B213" s="44"/>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A214" s="44"/>
-      <c r="B214" s="44"/>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A215" s="44"/>
-      <c r="B215" s="44"/>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A216" s="44"/>
-      <c r="B216" s="44"/>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A217" s="44"/>
-      <c r="B217" s="44"/>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A218" s="44"/>
-      <c r="B218" s="44"/>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A219" s="44"/>
-      <c r="B219" s="44"/>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A220" s="44"/>
-      <c r="B220" s="44"/>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A221" s="44"/>
-      <c r="B221" s="44"/>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A222" s="44"/>
-      <c r="B222" s="44"/>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A223" s="44"/>
-      <c r="B223" s="44"/>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A224" s="44"/>
-      <c r="B224" s="44"/>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A225" s="44"/>
-      <c r="B225" s="44"/>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A226" s="44"/>
-      <c r="B226" s="44"/>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A227" s="44"/>
-      <c r="B227" s="44"/>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A228" s="44"/>
-      <c r="B228" s="44"/>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" s="44"/>
-      <c r="B229" s="44"/>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" s="44"/>
-      <c r="B230" s="44"/>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A231" s="44"/>
-      <c r="B231" s="44"/>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A232" s="44"/>
-      <c r="B232" s="44"/>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A233" s="44"/>
-      <c r="B233" s="44"/>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A234" s="44"/>
-      <c r="B234" s="44"/>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A235" s="44"/>
-      <c r="B235" s="44"/>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A236" s="44"/>
-      <c r="B236" s="44"/>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A237" s="44"/>
-      <c r="B237" s="44"/>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A238" s="44"/>
-      <c r="B238" s="44"/>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A239" s="44"/>
-      <c r="B239" s="44"/>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A240" s="44"/>
-      <c r="B240" s="44"/>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A241" s="44"/>
-      <c r="B241" s="44"/>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A242" s="44"/>
-      <c r="B242" s="44"/>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A243" s="44"/>
-      <c r="B243" s="44"/>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A244" s="44"/>
-      <c r="B244" s="44"/>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A245" s="44"/>
-      <c r="B245" s="44"/>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A246" s="44"/>
-      <c r="B246" s="44"/>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A247" s="44"/>
-      <c r="B247" s="44"/>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A248" s="44"/>
-      <c r="B248" s="44"/>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A249" s="44"/>
-      <c r="B249" s="44"/>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A250" s="44"/>
-      <c r="B250" s="44"/>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A251" s="44"/>
-      <c r="B251" s="44"/>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A252" s="44"/>
-      <c r="B252" s="44"/>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A253" s="44"/>
-      <c r="B253" s="44"/>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A254" s="44"/>
-      <c r="B254" s="44"/>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A255" s="44"/>
-      <c r="B255" s="44"/>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A256" s="44"/>
-      <c r="B256" s="44"/>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A257" s="44"/>
-      <c r="B257" s="44"/>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A258" s="44"/>
-      <c r="B258" s="44"/>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A259" s="44"/>
-      <c r="B259" s="44"/>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A260" s="44"/>
-      <c r="B260" s="44"/>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A261" s="44"/>
-      <c r="B261" s="44"/>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A262" s="44"/>
-      <c r="B262" s="44"/>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A263" s="44"/>
-      <c r="B263" s="44"/>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A264" s="44"/>
-      <c r="B264" s="44"/>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A265" s="44"/>
-      <c r="B265" s="44"/>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A266" s="44"/>
-      <c r="B266" s="44"/>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A267" s="44"/>
-      <c r="B267" s="44"/>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A268" s="44"/>
-      <c r="B268" s="44"/>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A269" s="44"/>
-      <c r="B269" s="44"/>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A270" s="44"/>
-      <c r="B270" s="44"/>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A271" s="44"/>
-      <c r="B271" s="44"/>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A272" s="44"/>
-      <c r="B272" s="44"/>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A273" s="44"/>
-      <c r="B273" s="44"/>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A274" s="44"/>
-      <c r="B274" s="44"/>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" s="44"/>
-      <c r="B275" s="44"/>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A276" s="44"/>
-      <c r="B276" s="44"/>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" s="44"/>
-      <c r="B277" s="44"/>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A278" s="44"/>
-      <c r="B278" s="44"/>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A279" s="44"/>
-      <c r="B279" s="44"/>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" s="44"/>
-      <c r="B280" s="44"/>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A281" s="44"/>
-      <c r="B281" s="44"/>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A282" s="44"/>
-      <c r="B282" s="44"/>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A283" s="44"/>
-      <c r="B283" s="44"/>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A284" s="44"/>
-      <c r="B284" s="44"/>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A285" s="44"/>
-      <c r="B285" s="44"/>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A286" s="44"/>
-      <c r="B286" s="44"/>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A287" s="44"/>
-      <c r="B287" s="44"/>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A288" s="44"/>
-      <c r="B288" s="44"/>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A289" s="44"/>
-      <c r="B289" s="44"/>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A290" s="44"/>
-      <c r="B290" s="44"/>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A291" s="44"/>
-      <c r="B291" s="44"/>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A292" s="44"/>
-      <c r="B292" s="44"/>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A293" s="44"/>
-      <c r="B293" s="44"/>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A294" s="44"/>
-      <c r="B294" s="44"/>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A295" s="44"/>
-      <c r="B295" s="44"/>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A296" s="44"/>
-      <c r="B296" s="44"/>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A297" s="44"/>
-      <c r="B297" s="44"/>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A298" s="44"/>
-      <c r="B298" s="44"/>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A299" s="44"/>
-      <c r="B299" s="44"/>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A300" s="44"/>
-      <c r="B300" s="44"/>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A301" s="44"/>
-      <c r="B301" s="44"/>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A302" s="44"/>
-      <c r="B302" s="44"/>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A303" s="44"/>
-      <c r="B303" s="44"/>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A304" s="44"/>
-      <c r="B304" s="44"/>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A305" s="44"/>
-      <c r="B305" s="44"/>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A306" s="44"/>
-      <c r="B306" s="44"/>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A307" s="44"/>
-      <c r="B307" s="44"/>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A308" s="44"/>
-      <c r="B308" s="44"/>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A309" s="44"/>
-      <c r="B309" s="44"/>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A310" s="44"/>
-      <c r="B310" s="44"/>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A311" s="44"/>
-      <c r="B311" s="44"/>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A312" s="44"/>
-      <c r="B312" s="44"/>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A313" s="44"/>
-      <c r="B313" s="44"/>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A314" s="44"/>
-      <c r="B314" s="44"/>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A315" s="44"/>
-      <c r="B315" s="44"/>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A316" s="44"/>
-      <c r="B316" s="44"/>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A317" s="44"/>
-      <c r="B317" s="44"/>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A318" s="44"/>
-      <c r="B318" s="44"/>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A319" s="44"/>
-      <c r="B319" s="44"/>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A320" s="44"/>
-      <c r="B320" s="44"/>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A321" s="44"/>
-      <c r="B321" s="44"/>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A322" s="44"/>
-      <c r="B322" s="44"/>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A323" s="44"/>
-      <c r="B323" s="44"/>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A324" s="44"/>
-      <c r="B324" s="44"/>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A325" s="44"/>
-      <c r="B325" s="44"/>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A326" s="44"/>
-      <c r="B326" s="44"/>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A327" s="44"/>
-      <c r="B327" s="44"/>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A328" s="44"/>
-      <c r="B328" s="44"/>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A329" s="44"/>
-      <c r="B329" s="44"/>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A330" s="44"/>
-      <c r="B330" s="44"/>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A331" s="44"/>
-      <c r="B331" s="44"/>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A332" s="44"/>
-      <c r="B332" s="44"/>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A333" s="44"/>
-      <c r="B333" s="44"/>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A334" s="44"/>
-      <c r="B334" s="44"/>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A335" s="44"/>
-      <c r="B335" s="44"/>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A336" s="44"/>
-      <c r="B336" s="44"/>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A337" s="44"/>
-      <c r="B337" s="44"/>
-    </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A338" s="44"/>
-      <c r="B338" s="44"/>
-    </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A339" s="44"/>
-      <c r="B339" s="44"/>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A340" s="44"/>
-      <c r="B340" s="44"/>
-    </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A341" s="44"/>
-      <c r="B341" s="44"/>
-    </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A342" s="44"/>
-      <c r="B342" s="44"/>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A343" s="44"/>
-      <c r="B343" s="44"/>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A344" s="44"/>
-      <c r="B344" s="44"/>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A345" s="44"/>
-      <c r="B345" s="44"/>
-    </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A346" s="44"/>
-      <c r="B346" s="44"/>
-    </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A347" s="44"/>
-      <c r="B347" s="44"/>
-    </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A348" s="44"/>
-      <c r="B348" s="44"/>
-    </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A349" s="44"/>
-      <c r="B349" s="44"/>
-    </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A350" s="44"/>
-      <c r="B350" s="44"/>
-    </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A351" s="44"/>
-      <c r="B351" s="44"/>
-    </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A352" s="44"/>
-      <c r="B352" s="44"/>
-    </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A353" s="44"/>
-      <c r="B353" s="44"/>
-    </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A354" s="44"/>
-      <c r="B354" s="44"/>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A355" s="44"/>
-      <c r="B355" s="44"/>
-    </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A356" s="44"/>
-      <c r="B356" s="44"/>
-    </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A357" s="44"/>
-      <c r="B357" s="44"/>
-    </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A358" s="44"/>
-      <c r="B358" s="44"/>
-    </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A359" s="44"/>
-      <c r="B359" s="44"/>
-    </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A360" s="44"/>
-      <c r="B360" s="44"/>
-    </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A361" s="44"/>
-      <c r="B361" s="44"/>
-    </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A362" s="44"/>
-      <c r="B362" s="44"/>
-    </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A363" s="44"/>
-      <c r="B363" s="44"/>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A364" s="44"/>
-      <c r="B364" s="44"/>
-    </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A365" s="44"/>
-      <c r="B365" s="44"/>
-    </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A366" s="44"/>
-      <c r="B366" s="44"/>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A367" s="44"/>
-      <c r="B367" s="44"/>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A368" s="44"/>
-      <c r="B368" s="44"/>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A369" s="44"/>
-      <c r="B369" s="44"/>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A370" s="44"/>
-      <c r="B370" s="44"/>
-    </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A371" s="44"/>
-      <c r="B371" s="44"/>
-    </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A372" s="44"/>
-      <c r="B372" s="44"/>
-    </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A373" s="44"/>
-      <c r="B373" s="44"/>
-    </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A374" s="44"/>
-      <c r="B374" s="44"/>
-    </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A375" s="44"/>
-      <c r="B375" s="44"/>
-    </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A376" s="44"/>
-      <c r="B376" s="44"/>
-    </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A377" s="44"/>
-      <c r="B377" s="44"/>
-    </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A378" s="44"/>
-      <c r="B378" s="44"/>
-    </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A379" s="44"/>
-      <c r="B379" s="44"/>
-    </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A380" s="44"/>
-      <c r="B380" s="44"/>
-    </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A381" s="44"/>
-      <c r="B381" s="44"/>
-    </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A382" s="44"/>
-      <c r="B382" s="44"/>
-    </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A383" s="44"/>
-      <c r="B383" s="44"/>
-    </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A384" s="44"/>
-      <c r="B384" s="44"/>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A385" s="44"/>
-      <c r="B385" s="44"/>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A386" s="44"/>
-      <c r="B386" s="44"/>
-    </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A387" s="44"/>
-      <c r="B387" s="44"/>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A388" s="44"/>
-      <c r="B388" s="44"/>
-    </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A389" s="44"/>
-      <c r="B389" s="44"/>
-    </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A390" s="44"/>
-      <c r="B390" s="44"/>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A391" s="44"/>
-      <c r="B391" s="44"/>
-    </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A392" s="44"/>
-      <c r="B392" s="44"/>
-    </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A393" s="44"/>
-      <c r="B393" s="44"/>
-    </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A394" s="44"/>
-      <c r="B394" s="44"/>
-    </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A395" s="44"/>
-      <c r="B395" s="44"/>
-    </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A396" s="44"/>
-      <c r="B396" s="44"/>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A397" s="44"/>
-      <c r="B397" s="44"/>
-    </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A398" s="44"/>
-      <c r="B398" s="44"/>
-    </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A399" s="44"/>
-      <c r="B399" s="44"/>
-    </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A400" s="44"/>
-      <c r="B400" s="44"/>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A401" s="44"/>
-      <c r="B401" s="44"/>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A402" s="44"/>
-      <c r="B402" s="44"/>
-    </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A403" s="44"/>
-      <c r="B403" s="44"/>
-    </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A404" s="44"/>
-      <c r="B404" s="44"/>
-    </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A405" s="44"/>
-      <c r="B405" s="44"/>
-    </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A406" s="44"/>
-      <c r="B406" s="44"/>
-    </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A407" s="44"/>
-      <c r="B407" s="44"/>
-    </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A408" s="44"/>
-      <c r="B408" s="44"/>
-    </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A409" s="44"/>
-      <c r="B409" s="44"/>
-    </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A410" s="44"/>
-      <c r="B410" s="44"/>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A411" s="44"/>
-      <c r="B411" s="44"/>
-    </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A412" s="44"/>
-      <c r="B412" s="44"/>
-    </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A413" s="44"/>
-      <c r="B413" s="44"/>
-    </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A414" s="44"/>
-      <c r="B414" s="44"/>
-    </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A415" s="44"/>
-      <c r="B415" s="44"/>
-    </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A416" s="44"/>
-      <c r="B416" s="44"/>
-    </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A417" s="44"/>
-      <c r="B417" s="44"/>
-    </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A418" s="44"/>
-      <c r="B418" s="44"/>
-    </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A419" s="44"/>
-      <c r="B419" s="44"/>
-    </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A420" s="44"/>
-      <c r="B420" s="44"/>
-    </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A421" s="44"/>
-      <c r="B421" s="44"/>
-    </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A422" s="44"/>
-      <c r="B422" s="44"/>
-    </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A423" s="44"/>
-      <c r="B423" s="44"/>
-    </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A424" s="44"/>
-      <c r="B424" s="44"/>
-    </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A425" s="44"/>
-      <c r="B425" s="44"/>
-    </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A426" s="44"/>
-      <c r="B426" s="44"/>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A427" s="44"/>
-      <c r="B427" s="44"/>
-    </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A428" s="44"/>
-      <c r="B428" s="44"/>
-    </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A429" s="44"/>
-      <c r="B429" s="44"/>
-    </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A430" s="44"/>
-      <c r="B430" s="44"/>
-    </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A431" s="44"/>
-      <c r="B431" s="44"/>
-    </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A432" s="44"/>
-      <c r="B432" s="44"/>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A433" s="44"/>
-      <c r="B433" s="44"/>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A434" s="44"/>
-      <c r="B434" s="44"/>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A435" s="44"/>
-      <c r="B435" s="44"/>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A436" s="44"/>
-      <c r="B436" s="44"/>
-    </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A437" s="44"/>
-      <c r="B437" s="44"/>
-    </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A438" s="44"/>
-      <c r="B438" s="44"/>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A439" s="44"/>
-      <c r="B439" s="44"/>
-    </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A440" s="44"/>
-      <c r="B440" s="44"/>
-    </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A441" s="44"/>
-      <c r="B441" s="44"/>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A442" s="44"/>
-      <c r="B442" s="44"/>
-    </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A443" s="44"/>
-      <c r="B443" s="44"/>
-    </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A444" s="44"/>
-      <c r="B444" s="44"/>
-    </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A445" s="44"/>
-      <c r="B445" s="44"/>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A446" s="44"/>
-      <c r="B446" s="44"/>
-    </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A447" s="44"/>
-      <c r="B447" s="44"/>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A448" s="44"/>
-      <c r="B448" s="44"/>
-    </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A449" s="44"/>
-      <c r="B449" s="44"/>
-    </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A450" s="44"/>
-      <c r="B450" s="44"/>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A451" s="44"/>
-      <c r="B451" s="44"/>
-    </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A452" s="44"/>
-      <c r="B452" s="44"/>
-    </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A453" s="44"/>
-      <c r="B453" s="44"/>
-    </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A454" s="44"/>
-      <c r="B454" s="44"/>
-    </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A455" s="44"/>
-      <c r="B455" s="44"/>
-    </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A456" s="44"/>
-      <c r="B456" s="44"/>
-    </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A457" s="44"/>
-      <c r="B457" s="44"/>
-    </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A458" s="44"/>
-      <c r="B458" s="44"/>
-    </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A459" s="44"/>
-      <c r="B459" s="44"/>
-    </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A460" s="44"/>
-      <c r="B460" s="44"/>
-    </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A461" s="44"/>
-      <c r="B461" s="44"/>
-    </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A462" s="44"/>
-      <c r="B462" s="44"/>
-    </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A463" s="44"/>
-      <c r="B463" s="44"/>
-    </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A464" s="44"/>
-      <c r="B464" s="44"/>
-    </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A465" s="44"/>
-      <c r="B465" s="44"/>
-    </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A466" s="44"/>
-      <c r="B466" s="44"/>
-    </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A467" s="44"/>
-      <c r="B467" s="44"/>
-    </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A468" s="44"/>
-      <c r="B468" s="44"/>
-    </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A469" s="44"/>
-      <c r="B469" s="44"/>
-    </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A470" s="44"/>
-      <c r="B470" s="44"/>
-    </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A471" s="44"/>
-      <c r="B471" s="44"/>
-    </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A472" s="44"/>
-      <c r="B472" s="44"/>
-    </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A473" s="44"/>
-      <c r="B473" s="44"/>
-    </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A474" s="44"/>
-      <c r="B474" s="44"/>
-    </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A475" s="44"/>
-      <c r="B475" s="44"/>
-    </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A476" s="44"/>
-      <c r="B476" s="44"/>
-    </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A477" s="44"/>
-      <c r="B477" s="44"/>
-    </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A478" s="44"/>
-      <c r="B478" s="44"/>
-    </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A479" s="44"/>
-      <c r="B479" s="44"/>
-    </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A480" s="44"/>
-      <c r="B480" s="44"/>
-    </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A481" s="44"/>
-      <c r="B481" s="44"/>
-    </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A482" s="44"/>
-      <c r="B482" s="44"/>
-    </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A483" s="44"/>
-      <c r="B483" s="44"/>
-    </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A484" s="44"/>
-      <c r="B484" s="44"/>
-    </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A485" s="44"/>
-      <c r="B485" s="44"/>
-    </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A486" s="44"/>
-      <c r="B486" s="44"/>
-    </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A487" s="44"/>
-      <c r="B487" s="44"/>
-    </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A488" s="44"/>
-      <c r="B488" s="44"/>
-    </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A489" s="44"/>
-      <c r="B489" s="44"/>
-    </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A490" s="44"/>
-      <c r="B490" s="44"/>
-    </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A491" s="44"/>
-      <c r="B491" s="44"/>
-    </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A492" s="44"/>
-      <c r="B492" s="44"/>
-    </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A493" s="44"/>
-      <c r="B493" s="44"/>
-    </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A494" s="44"/>
-      <c r="B494" s="44"/>
-    </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A495" s="44"/>
-      <c r="B495" s="44"/>
-    </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A496" s="44"/>
-      <c r="B496" s="44"/>
-    </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A497" s="44"/>
-      <c r="B497" s="44"/>
-    </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A498" s="44"/>
-      <c r="B498" s="44"/>
-    </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A499" s="44"/>
-      <c r="B499" s="44"/>
-    </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A500" s="44"/>
-      <c r="B500" s="44"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3B42F4-1841-984B-BE93-9807147BD0DF}">
-  <dimension ref="A1:K500"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1207</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1208</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1209</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1210</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1211</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1212</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1215</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2">
-        <v>202501</v>
-      </c>
-      <c r="D2">
-        <v>173399188</v>
-      </c>
-      <c r="E2">
-        <v>173399188</v>
-      </c>
-      <c r="F2">
-        <v>210675369</v>
-      </c>
-      <c r="G2">
-        <v>210675369</v>
-      </c>
-      <c r="H2">
-        <v>22320594</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>22320594</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>839</v>
-      </c>
-      <c r="C3">
-        <v>202501</v>
-      </c>
-      <c r="D3">
-        <v>436803319</v>
-      </c>
-      <c r="E3">
-        <v>436803319</v>
-      </c>
-      <c r="F3">
-        <v>512257135</v>
-      </c>
-      <c r="G3">
-        <v>512257135</v>
-      </c>
-      <c r="H3">
-        <v>69015494</v>
-      </c>
-      <c r="I3">
-        <v>-6</v>
-      </c>
-      <c r="J3">
-        <v>69015500</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C4">
-        <v>202501</v>
-      </c>
-      <c r="D4">
-        <v>1308582154</v>
-      </c>
-      <c r="E4">
-        <v>1308582154</v>
-      </c>
-      <c r="F4">
-        <v>1341478541</v>
-      </c>
-      <c r="G4">
-        <v>1341478541</v>
-      </c>
-      <c r="H4">
-        <v>32896387</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>32896387</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5">
-        <v>202501</v>
-      </c>
-      <c r="D5">
-        <v>32448805638</v>
-      </c>
-      <c r="E5">
-        <v>30676649972</v>
-      </c>
-      <c r="F5">
-        <v>39334196918</v>
-      </c>
-      <c r="G5">
-        <v>37562041252</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>1772155666</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6">
-        <v>202501</v>
-      </c>
-      <c r="D6">
-        <v>47590494159</v>
-      </c>
-      <c r="E6">
-        <v>45361868519</v>
-      </c>
-      <c r="F6">
-        <v>72082837725</v>
-      </c>
-      <c r="G6">
-        <v>69854212085</v>
-      </c>
-      <c r="H6">
-        <v>22477822788</v>
-      </c>
-      <c r="I6">
-        <v>2014520778</v>
-      </c>
-      <c r="J6">
-        <v>20463302010</v>
-      </c>
-      <c r="K6">
-        <v>2228625640</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>839</v>
-      </c>
-      <c r="C7">
-        <v>202501</v>
-      </c>
-      <c r="D7">
-        <v>5400889117</v>
-      </c>
-      <c r="E7">
-        <v>3407840127</v>
-      </c>
-      <c r="F7">
-        <v>5385171178</v>
-      </c>
-      <c r="G7">
-        <v>3392122188</v>
-      </c>
-      <c r="H7">
-        <v>-674093825</v>
-      </c>
-      <c r="I7">
-        <v>658375886</v>
-      </c>
-      <c r="J7">
-        <v>-1332469711</v>
-      </c>
-      <c r="K7">
-        <v>1993048990</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>1077</v>
-      </c>
-      <c r="C8">
-        <v>202501</v>
-      </c>
-      <c r="D8">
-        <v>303769141</v>
-      </c>
-      <c r="E8">
-        <v>303769141</v>
-      </c>
-      <c r="F8">
-        <v>492130820</v>
-      </c>
-      <c r="G8">
-        <v>492130820</v>
-      </c>
-      <c r="H8">
-        <v>188361679</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>188361679</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C9">
-        <v>202501</v>
-      </c>
-      <c r="D9">
-        <v>158252436</v>
-      </c>
-      <c r="E9">
-        <v>57071142</v>
-      </c>
-      <c r="F9">
-        <v>158748472</v>
-      </c>
-      <c r="G9">
-        <v>57567178</v>
-      </c>
-      <c r="H9">
-        <v>2469611</v>
-      </c>
-      <c r="I9">
-        <v>-1973575</v>
-      </c>
-      <c r="J9">
-        <v>4443186</v>
-      </c>
-      <c r="K9">
-        <v>101181294</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C10">
-        <v>202501</v>
-      </c>
-      <c r="D10">
-        <v>53021962</v>
-      </c>
-      <c r="E10">
-        <v>53021962</v>
-      </c>
-      <c r="F10">
-        <v>66253328</v>
-      </c>
-      <c r="G10">
-        <v>66253328</v>
-      </c>
-      <c r="H10">
-        <v>13231366</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>13231366</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>852</v>
-      </c>
-      <c r="C11">
-        <v>202501</v>
-      </c>
-      <c r="D11">
-        <v>1123643875</v>
-      </c>
-      <c r="E11">
-        <v>764972652</v>
-      </c>
-      <c r="F11">
-        <v>1422300938</v>
-      </c>
-      <c r="G11">
-        <v>1063629715</v>
-      </c>
-      <c r="H11">
-        <v>465607073</v>
-      </c>
-      <c r="I11">
-        <v>-166950010</v>
-      </c>
-      <c r="J11">
-        <v>632557083</v>
-      </c>
-      <c r="K11">
-        <v>358671223</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
-      <c r="B12" s="44"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
     </row>
@@ -60035,16 +60035,10 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -60057,10 +60051,16 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ab22448b-4c5c-4966-bbdb-d0c4a65bda1b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df0aad82-cca9-4ab3-a26b-b2d93ab652bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -60084,6 +60084,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -60099,20 +60115,4 @@
     <ds:schemaRef ds:uri="df0aad82-cca9-4ab3-a26b-b2d93ab652bf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>